<commit_message>
Added a new file reference
</commit_message>
<xml_diff>
--- a/DataNeeded.xlsx
+++ b/DataNeeded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezekiel Adebayo\Desktop\Statistics with R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43A34ED-AA55-44FE-BF65-A07663BFDAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0831869-3057-455A-9E8C-41ECEC33F25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{F9A033FA-32C5-4EC0-8640-8C0B424670D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F9A033FA-32C5-4EC0-8640-8C0B424670D7}"/>
   </bookViews>
   <sheets>
     <sheet name="1a-conception" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>Year of conception</t>
   </si>
@@ -685,26 +685,6 @@
       </rPr>
       <t xml:space="preserve"> 
 Number of conceptions terminated by abortion</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>All ages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Number of conceptions</t>
     </r>
   </si>
   <si>
@@ -2301,9 +2281,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2438,29 +2415,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2496,6 +2474,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="#,##0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3328,26 +3326,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0.0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4568,35 +4546,35 @@
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{FE4EB3CC-7F82-4676-8560-04228A9DD220}" name="Year of conception" dataDxfId="48" dataCellStyle="Normal 2 2 2"/>
     <tableColumn id="18" xr3:uid="{F843A42F-3669-4D28-9889-71E15C78C506}" name="Age under 20_x000a_Number of conceptions" dataDxfId="47" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="20" xr3:uid="{CF1AF1DC-CF22-4D00-B162-164F44F58D4B}" name="Age under 20_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="46" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="21" xr3:uid="{594196FE-10A0-4CFE-B629-D8C412D30E08}" name="Age under 20_x000a_Percentage of conceptions leading to abortion" dataDxfId="45" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="22" xr3:uid="{99D1DCF7-6015-4FBC-93D4-528A9CC202BD}" name="Age 20 to 24_x000a_Percentage of conceptions outside marriage or civil partnership " dataDxfId="44" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="23" xr3:uid="{7F3BA439-5FA0-4D8F-9953-64445515732D}" name="Age 20 to 24_x000a_Number of conceptions" dataDxfId="43" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="25" xr3:uid="{96C5C68D-14E9-4050-B88B-EF2AC5061DCB}" name="Age 20 to 24_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="42" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="26" xr3:uid="{93C6673E-EA22-4A55-8D6D-7BF552CECA52}" name="Age 20 to 24_x000a_Percentage of conceptions leading to abortion" dataDxfId="41" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="27" xr3:uid="{711C3F3E-9C68-4A94-BD88-7659D5B70D49}" name="Age 25 to 29_x000a_Percentage of conceptions outside marriage or civil partnership" dataDxfId="40" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="28" xr3:uid="{3C22E9FC-8A91-4627-A061-5C40F0CDEA46}" name="Age 25 to 29_x000a_Number of conceptions" dataDxfId="39" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="30" xr3:uid="{4DDC8FF9-22B3-4095-B9B7-A848815290A0}" name="Age 25 to 29_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="38" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="31" xr3:uid="{65553446-D18E-4AD5-AC56-226E82D9C1D2}" name="Age 25 to 29_x000a_Percentage of conceptions leading to abortion" dataDxfId="37" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="32" xr3:uid="{D3DE77EE-A451-493C-919C-03083EA623EF}" name="Age 30 to 34_x000a_Percentage of conceptions outside marriage or civil partnership" dataDxfId="36" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="33" xr3:uid="{6481769D-871E-4D99-B8B0-C822935994A1}" name="Age 30 to 34_x000a_Number of conceptions" dataDxfId="35" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="35" xr3:uid="{993EE2B6-3FFA-47D5-BECE-59C4078241AD}" name="Age 30 to 34_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="34" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="36" xr3:uid="{85747303-85E6-4A3C-8331-02D1B5A0F0D9}" name="Age 30 to 34_x000a_Percentage of conceptions leading to abortion" dataDxfId="33" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="37" xr3:uid="{D65AB0BE-7A9D-4103-BF8F-65A485799436}" name="Age 35 to 39_x000a_Percentage of conceptions outside marriage or civil partnership " dataDxfId="32" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="38" xr3:uid="{57E43F04-633D-450B-A6A1-6589AFCA2016}" name="Age 35 to 39_x000a_Number of conceptions" dataDxfId="31" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="40" xr3:uid="{6882C9D9-EF09-473B-BB4E-071A1C7F271C}" name="Age 35 to 39_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership " dataDxfId="30" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="41" xr3:uid="{BB240C2B-8077-4303-BD03-E57B2990F306}" name="Age 35 to 39 Percentage of conceptions leading to abortion" dataDxfId="29" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="42" xr3:uid="{032B815C-7743-40DE-80CD-8BF088874FAF}" name="Age 40 and over_x000a_Percentage of conceptions outside marriage or civil partnership" dataDxfId="28" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="43" xr3:uid="{308012AC-40CB-4D10-B049-3CFBE86D20FD}" name="Age 40 and over_x000a_Number of conceptions" dataDxfId="27" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="45" xr3:uid="{5BD7E29D-577D-4BB3-92EA-D9C085C01AC8}" name="Age 40 and over_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="26" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="46" xr3:uid="{B1D050C0-86B8-4507-94FE-FDF53219208B}" name="Age 40 and over_x000a_Percentage of conceptions leading to abortion" dataDxfId="25" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="20" xr3:uid="{CF1AF1DC-CF22-4D00-B162-164F44F58D4B}" name="Age under 20_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="2" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="21" xr3:uid="{594196FE-10A0-4CFE-B629-D8C412D30E08}" name="Age under 20_x000a_Percentage of conceptions leading to abortion" dataDxfId="46" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="22" xr3:uid="{99D1DCF7-6015-4FBC-93D4-528A9CC202BD}" name="Age 20 to 24_x000a_Percentage of conceptions outside marriage or civil partnership " dataDxfId="45" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="23" xr3:uid="{7F3BA439-5FA0-4D8F-9953-64445515732D}" name="Age 20 to 24_x000a_Number of conceptions" dataDxfId="44" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="25" xr3:uid="{96C5C68D-14E9-4050-B88B-EF2AC5061DCB}" name="Age 20 to 24_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="43" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="26" xr3:uid="{93C6673E-EA22-4A55-8D6D-7BF552CECA52}" name="Age 20 to 24_x000a_Percentage of conceptions leading to abortion" dataDxfId="42" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="27" xr3:uid="{711C3F3E-9C68-4A94-BD88-7659D5B70D49}" name="Age 25 to 29_x000a_Percentage of conceptions outside marriage or civil partnership" dataDxfId="41" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="28" xr3:uid="{3C22E9FC-8A91-4627-A061-5C40F0CDEA46}" name="Age 25 to 29_x000a_Number of conceptions" dataDxfId="40" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="30" xr3:uid="{4DDC8FF9-22B3-4095-B9B7-A848815290A0}" name="Age 25 to 29_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="39" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="31" xr3:uid="{65553446-D18E-4AD5-AC56-226E82D9C1D2}" name="Age 25 to 29_x000a_Percentage of conceptions leading to abortion" dataDxfId="38" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="32" xr3:uid="{D3DE77EE-A451-493C-919C-03083EA623EF}" name="Age 30 to 34_x000a_Percentage of conceptions outside marriage or civil partnership" dataDxfId="37" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="33" xr3:uid="{6481769D-871E-4D99-B8B0-C822935994A1}" name="Age 30 to 34_x000a_Number of conceptions" dataDxfId="36" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="35" xr3:uid="{993EE2B6-3FFA-47D5-BECE-59C4078241AD}" name="Age 30 to 34_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="35" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="36" xr3:uid="{85747303-85E6-4A3C-8331-02D1B5A0F0D9}" name="Age 30 to 34_x000a_Percentage of conceptions leading to abortion" dataDxfId="34" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="37" xr3:uid="{D65AB0BE-7A9D-4103-BF8F-65A485799436}" name="Age 35 to 39_x000a_Percentage of conceptions outside marriage or civil partnership " dataDxfId="33" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="38" xr3:uid="{57E43F04-633D-450B-A6A1-6589AFCA2016}" name="Age 35 to 39_x000a_Number of conceptions" dataDxfId="32" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="40" xr3:uid="{6882C9D9-EF09-473B-BB4E-071A1C7F271C}" name="Age 35 to 39_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership " dataDxfId="31" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="41" xr3:uid="{BB240C2B-8077-4303-BD03-E57B2990F306}" name="Age 35 to 39 Percentage of conceptions leading to abortion" dataDxfId="30" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="42" xr3:uid="{032B815C-7743-40DE-80CD-8BF088874FAF}" name="Age 40 and over_x000a_Percentage of conceptions outside marriage or civil partnership" dataDxfId="29" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="43" xr3:uid="{308012AC-40CB-4D10-B049-3CFBE86D20FD}" name="Age 40 and over_x000a_Number of conceptions" dataDxfId="28" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="45" xr3:uid="{5BD7E29D-577D-4BB3-92EA-D9C085C01AC8}" name="Age 40 and over_x000a_Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership" dataDxfId="27" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="46" xr3:uid="{B1D050C0-86B8-4507-94FE-FDF53219208B}" name="Age 40 and over_x000a_Percentage of conceptions leading to abortion" dataDxfId="26" dataCellStyle="Normal 2 2 2"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E50AD4A7-C20F-4A08-BB36-191AD6FBBDEC}" name="Table413" displayName="Table413" ref="A1:T13" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E50AD4A7-C20F-4A08-BB36-191AD6FBBDEC}" name="Table413" displayName="Table413" ref="A1:T13" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A1:T13" xr:uid="{6E5B5B3E-A8A4-4AA9-9ABA-5E982384B055}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4620,26 +4598,26 @@
     <filterColumn colId="19" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="2" xr3:uid="{E7BA53E8-E711-4627-A303-862B790822AE}" name="Name" dataDxfId="21" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="3" xr3:uid="{FEB5BBA8-829B-4517-8FA3-ECEB3B34B1CF}" name="Geography" dataDxfId="20" dataCellStyle="Normal 2 2 2"/>
-    <tableColumn id="4" xr3:uid="{039DC26F-DBA1-4016-818C-D52F0A653303}" name="All ages _x000a_Number of conceptions" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{24C9CAB7-4A6B-4A12-83EE-64036B11E5D7}" name="All ages _x000a_Percentage of conceptions leading to abortion" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{17EC1AB4-1E46-4996-BCB9-A5774994FA3B}" name="Age Under 16 _x000a_Number of conceptions" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{92EAD359-7BA1-4AFB-9DCD-3B7D3EFBFF77}" name="Age Under 16 _x000a_Percentage of conceptions leading to abortion" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{2E5669A9-A0ED-40F7-A57C-1FCAC7B1B77D}" name="Age Under 18 _x000a_Number of conceptions" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{B8B46338-A053-4047-8F7B-0C87AD29F7CC}" name="Age Under 18 _x000a_Percentage of conceptions leading to abortion" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{9070F7A3-B4BF-4933-897F-9AD02B51BF5B}" name="Age under 20 _x000a_Number of conceptions" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{FDDE8E35-0823-46FB-976D-37945A36F6CE}" name="Age under 20 _x000a_Percentage of conceptions leading to abortion" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{48376CBA-ADF8-47AA-852B-3CAC4D12CC75}" name="Age 20 to 24 _x000a_Number of conceptions" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{FCADCB3E-512A-4254-A70E-EFC7DAC48C1B}" name="Age 20 to 24 _x000a_Percentage of conceptions leading to abortion" dataDxfId="10"/>
-    <tableColumn id="24" xr3:uid="{202FE732-56AF-43DF-9F57-EC415424ED8F}" name="Age 25 to 29 _x000a_Number of conceptions" dataDxfId="9"/>
-    <tableColumn id="26" xr3:uid="{3E519CAB-2EA3-46DB-A5E7-EFDA795FF02C}" name="Age 25 to 29 _x000a_Percentage of conceptions leading to abortion" dataDxfId="8"/>
-    <tableColumn id="28" xr3:uid="{29E83D7F-0998-4596-AD94-DF5F2AF78ADB}" name="Age 30 to 34 _x000a_Number of conceptions" dataDxfId="7"/>
-    <tableColumn id="30" xr3:uid="{0343FF93-2697-4363-97D4-CF65F6FF1350}" name="Age 30 to 34 _x000a_Percentage of conceptions leading to abortion" dataDxfId="6"/>
-    <tableColumn id="32" xr3:uid="{A1324F87-16A1-4297-B897-20F038812534}" name="Age 35 to 39 _x000a_Number of conceptions" dataDxfId="5"/>
-    <tableColumn id="34" xr3:uid="{A2ACA874-A417-4B2D-BAF6-E0D827CDF638}" name="Age 35 to 39 _x000a_Percentage of conceptions leading to abortion" dataDxfId="4"/>
-    <tableColumn id="36" xr3:uid="{B782151B-6683-42AF-AA53-40240E9B7D2D}" name="Age 40 and over _x000a_Number of conceptions" dataDxfId="3"/>
-    <tableColumn id="38" xr3:uid="{1F307859-5B4A-4AE8-8F65-C8DA2E91E49B}" name="Age 40 and over _x000a_Percentage of conceptions leading to abortion" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E7BA53E8-E711-4627-A303-862B790822AE}" name="Name" dataDxfId="22" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="3" xr3:uid="{FEB5BBA8-829B-4517-8FA3-ECEB3B34B1CF}" name="Geography" dataDxfId="21" dataCellStyle="Normal 2 2 2"/>
+    <tableColumn id="4" xr3:uid="{039DC26F-DBA1-4016-818C-D52F0A653303}" name="All ages _x000a_Number of conceptions" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{24C9CAB7-4A6B-4A12-83EE-64036B11E5D7}" name="All ages _x000a_Percentage of conceptions leading to abortion" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{17EC1AB4-1E46-4996-BCB9-A5774994FA3B}" name="Age Under 16 _x000a_Number of conceptions" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{92EAD359-7BA1-4AFB-9DCD-3B7D3EFBFF77}" name="Age Under 16 _x000a_Percentage of conceptions leading to abortion" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{2E5669A9-A0ED-40F7-A57C-1FCAC7B1B77D}" name="Age Under 18 _x000a_Number of conceptions" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{B8B46338-A053-4047-8F7B-0C87AD29F7CC}" name="Age Under 18 _x000a_Percentage of conceptions leading to abortion" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{9070F7A3-B4BF-4933-897F-9AD02B51BF5B}" name="Age under 20 _x000a_Number of conceptions" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{FDDE8E35-0823-46FB-976D-37945A36F6CE}" name="Age under 20 _x000a_Percentage of conceptions leading to abortion" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{48376CBA-ADF8-47AA-852B-3CAC4D12CC75}" name="Age 20 to 24 _x000a_Number of conceptions" dataDxfId="12"/>
+    <tableColumn id="22" xr3:uid="{FCADCB3E-512A-4254-A70E-EFC7DAC48C1B}" name="Age 20 to 24 _x000a_Percentage of conceptions leading to abortion" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{202FE732-56AF-43DF-9F57-EC415424ED8F}" name="Age 25 to 29 _x000a_Number of conceptions" dataDxfId="10"/>
+    <tableColumn id="26" xr3:uid="{3E519CAB-2EA3-46DB-A5E7-EFDA795FF02C}" name="Age 25 to 29 _x000a_Percentage of conceptions leading to abortion" dataDxfId="9"/>
+    <tableColumn id="28" xr3:uid="{29E83D7F-0998-4596-AD94-DF5F2AF78ADB}" name="Age 30 to 34 _x000a_Number of conceptions" dataDxfId="8"/>
+    <tableColumn id="30" xr3:uid="{0343FF93-2697-4363-97D4-CF65F6FF1350}" name="Age 30 to 34 _x000a_Percentage of conceptions leading to abortion" dataDxfId="7"/>
+    <tableColumn id="32" xr3:uid="{A1324F87-16A1-4297-B897-20F038812534}" name="Age 35 to 39 _x000a_Number of conceptions" dataDxfId="6"/>
+    <tableColumn id="34" xr3:uid="{A2ACA874-A417-4B2D-BAF6-E0D827CDF638}" name="Age 35 to 39 _x000a_Percentage of conceptions leading to abortion" dataDxfId="5"/>
+    <tableColumn id="36" xr3:uid="{B782151B-6683-42AF-AA53-40240E9B7D2D}" name="Age 40 and over _x000a_Number of conceptions" dataDxfId="4"/>
+    <tableColumn id="38" xr3:uid="{1F307859-5B4A-4AE8-8F65-C8DA2E91E49B}" name="Age 40 and over _x000a_Percentage of conceptions leading to abortion" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6167,8 +6145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A093282-0E65-4553-B1F2-157F17C747C1}">
   <dimension ref="A1:BH51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AZ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1:BC1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB8" sqref="BB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10059,1150 +10037,1055 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAD412E-1ADA-4742-8F14-530D7BF15C09}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:AG1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="15.61328125" style="70" customWidth="1"/>
-    <col min="15" max="16384" width="9.07421875" style="70"/>
+    <col min="1" max="13" width="15.61328125" style="69" customWidth="1"/>
+    <col min="14" max="16384" width="9.07421875" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="121" t="s">
+    <row r="1" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="121" t="s">
         <v>34</v>
       </c>
       <c r="C1" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="121" t="s">
         <v>36</v>
       </c>
       <c r="E1" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="123" t="s">
+      <c r="H1" s="121" t="s">
         <v>40</v>
       </c>
       <c r="I1" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="123" t="s">
+      <c r="J1" s="121" t="s">
         <v>42</v>
       </c>
       <c r="K1" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="122" t="s">
+      <c r="M1" s="123" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="124" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="71"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="125">
+      <c r="N1" s="70"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="124">
         <v>2020</v>
       </c>
-      <c r="B2" s="16">
-        <v>316616</v>
-      </c>
-      <c r="C2" s="98">
+      <c r="B2" s="97">
         <v>1077</v>
       </c>
-      <c r="D2" s="17">
+      <c r="C2" s="17">
         <v>14.7</v>
       </c>
-      <c r="E2" s="98">
+      <c r="D2" s="97">
         <v>17896</v>
       </c>
-      <c r="F2" s="17">
+      <c r="E2" s="17">
         <v>9.5</v>
       </c>
-      <c r="G2" s="98">
+      <c r="F2" s="97">
         <v>77219</v>
       </c>
-      <c r="H2" s="17">
+      <c r="G2" s="17">
         <v>7.4</v>
       </c>
-      <c r="I2" s="98">
+      <c r="H2" s="97">
         <v>131586</v>
       </c>
-      <c r="J2" s="17">
+      <c r="I2" s="17">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K2" s="98">
+      <c r="J2" s="97">
         <v>73236</v>
       </c>
-      <c r="L2" s="17">
+      <c r="K2" s="17">
         <v>14.1</v>
       </c>
-      <c r="M2" s="98">
+      <c r="L2" s="97">
         <v>15602</v>
       </c>
-      <c r="N2" s="18">
+      <c r="M2" s="18">
         <v>27.8</v>
       </c>
-      <c r="O2" s="71"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="94">
+      <c r="N2" s="70"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="93">
         <v>2019</v>
       </c>
-      <c r="B3" s="22">
-        <v>329997</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="B3" s="19">
         <v>1281</v>
       </c>
-      <c r="D3" s="58">
+      <c r="C3" s="58">
         <v>13</v>
       </c>
-      <c r="E3" s="19">
+      <c r="D3" s="19">
         <v>20005</v>
       </c>
-      <c r="F3" s="58">
+      <c r="E3" s="58">
         <v>8</v>
       </c>
-      <c r="G3" s="19">
+      <c r="F3" s="19">
         <v>86031</v>
       </c>
-      <c r="H3" s="20">
+      <c r="G3" s="20">
         <v>7.1</v>
       </c>
-      <c r="I3" s="19">
+      <c r="H3" s="19">
         <v>133659</v>
       </c>
-      <c r="J3" s="20">
+      <c r="I3" s="20">
         <v>8.1</v>
       </c>
-      <c r="K3" s="19">
+      <c r="J3" s="19">
         <v>73566</v>
       </c>
-      <c r="L3" s="20">
+      <c r="K3" s="20">
         <v>13.1</v>
       </c>
-      <c r="M3" s="19">
+      <c r="L3" s="19">
         <v>15450</v>
       </c>
-      <c r="N3" s="23">
+      <c r="M3" s="23">
         <v>24.9</v>
       </c>
-      <c r="O3" s="71"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="94">
+      <c r="N3" s="70"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="93">
         <v>2018</v>
       </c>
-      <c r="B4" s="29">
-        <v>341122</v>
-      </c>
-      <c r="C4" s="74">
+      <c r="B4" s="73">
         <v>1432</v>
       </c>
-      <c r="D4" s="126">
+      <c r="C4" s="125">
         <v>11.6</v>
       </c>
-      <c r="E4" s="74">
+      <c r="D4" s="73">
         <v>21450</v>
       </c>
-      <c r="F4" s="126">
+      <c r="E4" s="125">
         <v>7.4</v>
       </c>
-      <c r="G4" s="74">
+      <c r="F4" s="73">
         <v>89938</v>
       </c>
-      <c r="H4" s="126">
+      <c r="G4" s="125">
         <v>6.7</v>
       </c>
-      <c r="I4" s="74">
+      <c r="H4" s="73">
         <v>138482</v>
       </c>
-      <c r="J4" s="126">
+      <c r="I4" s="125">
         <v>7.5</v>
       </c>
-      <c r="K4" s="74">
+      <c r="J4" s="73">
         <v>74723</v>
       </c>
-      <c r="L4" s="126">
+      <c r="K4" s="125">
         <v>12.4</v>
       </c>
-      <c r="M4" s="74">
+      <c r="L4" s="73">
         <v>15096</v>
       </c>
-      <c r="N4" s="127">
+      <c r="M4" s="126">
         <v>24.4</v>
       </c>
-      <c r="O4" s="71"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="94">
+      <c r="N4" s="70"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="93">
         <v>2017</v>
       </c>
-      <c r="B5" s="128">
-        <v>350158</v>
-      </c>
-      <c r="C5" s="74">
+      <c r="B5" s="73">
         <v>1428</v>
       </c>
-      <c r="D5" s="126">
+      <c r="C5" s="125">
         <v>10.5</v>
       </c>
-      <c r="E5" s="74">
+      <c r="D5" s="73">
         <v>22003</v>
       </c>
-      <c r="F5" s="126">
+      <c r="E5" s="125">
         <v>7.1</v>
       </c>
-      <c r="G5" s="74">
+      <c r="F5" s="73">
         <v>95327</v>
       </c>
-      <c r="H5" s="126">
+      <c r="G5" s="125">
         <v>6.4</v>
       </c>
-      <c r="I5" s="74">
+      <c r="H5" s="73">
         <v>140701</v>
       </c>
-      <c r="J5" s="126">
+      <c r="I5" s="125">
         <v>7.2</v>
       </c>
-      <c r="K5" s="74">
+      <c r="J5" s="73">
         <v>75477</v>
       </c>
-      <c r="L5" s="126">
+      <c r="K5" s="125">
         <v>11.6</v>
       </c>
-      <c r="M5" s="74">
+      <c r="L5" s="73">
         <v>15164</v>
       </c>
-      <c r="N5" s="127">
+      <c r="M5" s="126">
         <v>22.8</v>
       </c>
-      <c r="O5" s="71"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="94">
+      <c r="N5" s="70"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="93">
         <v>2016</v>
       </c>
-      <c r="B6" s="128">
-        <v>364339</v>
-      </c>
-      <c r="C6" s="74">
+      <c r="B6" s="73">
         <v>1580</v>
       </c>
-      <c r="D6" s="126">
+      <c r="C6" s="125">
         <v>8.9</v>
       </c>
-      <c r="E6" s="76">
+      <c r="D6" s="75">
         <v>23800</v>
       </c>
-      <c r="F6" s="129">
+      <c r="E6" s="127">
         <v>6.8</v>
       </c>
-      <c r="G6" s="76">
+      <c r="F6" s="75">
         <v>102642</v>
       </c>
-      <c r="H6" s="129">
+      <c r="G6" s="127">
         <v>6</v>
       </c>
-      <c r="I6" s="76">
+      <c r="H6" s="75">
         <v>145141</v>
       </c>
-      <c r="J6" s="129">
+      <c r="I6" s="127">
         <v>6.8</v>
       </c>
-      <c r="K6" s="76">
+      <c r="J6" s="75">
         <v>75806</v>
       </c>
-      <c r="L6" s="129">
+      <c r="K6" s="127">
         <v>11</v>
       </c>
-      <c r="M6" s="74">
+      <c r="L6" s="73">
         <v>15370</v>
       </c>
-      <c r="N6" s="130">
+      <c r="M6" s="128">
         <v>21.7</v>
       </c>
-      <c r="O6" s="71"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="94">
+      <c r="N6" s="70"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="93">
         <v>2015</v>
       </c>
-      <c r="B7" s="128">
-        <v>374346</v>
-      </c>
-      <c r="C7" s="74">
+      <c r="B7" s="73">
         <v>1633</v>
       </c>
-      <c r="D7" s="131">
+      <c r="C7" s="129">
         <v>9.6</v>
       </c>
-      <c r="E7" s="74">
+      <c r="D7" s="73">
         <v>25526</v>
       </c>
-      <c r="F7" s="131">
+      <c r="E7" s="129">
         <v>6.8</v>
       </c>
-      <c r="G7" s="74">
+      <c r="F7" s="73">
         <v>108125</v>
       </c>
-      <c r="H7" s="131">
+      <c r="G7" s="129">
         <v>6</v>
       </c>
-      <c r="I7" s="74">
+      <c r="H7" s="73">
         <v>148198</v>
       </c>
-      <c r="J7" s="131">
+      <c r="I7" s="129">
         <v>6.4</v>
       </c>
-      <c r="K7" s="74">
+      <c r="J7" s="73">
         <v>75203</v>
       </c>
-      <c r="L7" s="131">
+      <c r="K7" s="129">
         <v>10.6</v>
       </c>
-      <c r="M7" s="74">
+      <c r="L7" s="73">
         <v>15661</v>
       </c>
-      <c r="N7" s="130">
+      <c r="M7" s="128">
         <v>22.1</v>
       </c>
-      <c r="O7" s="71"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="94">
+      <c r="N7" s="70"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="93">
         <v>2014</v>
       </c>
-      <c r="B8" s="132">
-        <v>371511</v>
-      </c>
-      <c r="C8" s="76">
+      <c r="B8" s="75">
         <v>1687</v>
       </c>
-      <c r="D8" s="129">
+      <c r="C8" s="127">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E8" s="76">
+      <c r="D8" s="75">
         <v>27160</v>
       </c>
-      <c r="F8" s="129">
+      <c r="E8" s="127">
         <v>7</v>
       </c>
-      <c r="G8" s="76">
+      <c r="F8" s="75">
         <v>109933</v>
       </c>
-      <c r="H8" s="129">
+      <c r="G8" s="127">
         <v>6.1</v>
       </c>
-      <c r="I8" s="74">
+      <c r="H8" s="73">
         <v>146423</v>
       </c>
-      <c r="J8" s="131">
+      <c r="I8" s="129">
         <v>6.4</v>
       </c>
-      <c r="K8" s="76">
+      <c r="J8" s="75">
         <v>71014</v>
       </c>
-      <c r="L8" s="129">
+      <c r="K8" s="127">
         <v>10.5</v>
       </c>
-      <c r="M8" s="76">
+      <c r="L8" s="75">
         <v>15294</v>
       </c>
-      <c r="N8" s="133">
+      <c r="M8" s="130">
         <v>22.1</v>
       </c>
-      <c r="O8" s="71"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="94">
+      <c r="N8" s="70"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="93">
         <v>2013</v>
       </c>
-      <c r="B9" s="132">
-        <v>373371</v>
-      </c>
-      <c r="C9" s="76">
+      <c r="B9" s="75">
         <v>1746</v>
       </c>
-      <c r="D9" s="129">
+      <c r="C9" s="127">
         <v>10.1</v>
       </c>
-      <c r="E9" s="76">
+      <c r="D9" s="75">
         <v>29825</v>
       </c>
-      <c r="F9" s="129">
+      <c r="E9" s="127">
         <v>7.2</v>
       </c>
-      <c r="G9" s="74">
+      <c r="F9" s="73">
         <v>111845</v>
       </c>
-      <c r="H9" s="131">
+      <c r="G9" s="129">
         <v>6.1</v>
       </c>
-      <c r="I9" s="76">
+      <c r="H9" s="75">
         <v>144971</v>
       </c>
-      <c r="J9" s="129">
+      <c r="I9" s="127">
         <v>6.2</v>
       </c>
-      <c r="K9" s="76">
+      <c r="J9" s="75">
         <v>69557</v>
       </c>
-      <c r="L9" s="129">
+      <c r="K9" s="127">
         <v>10.3</v>
       </c>
-      <c r="M9" s="76">
+      <c r="L9" s="75">
         <v>15427</v>
       </c>
-      <c r="N9" s="133">
+      <c r="M9" s="130">
         <v>22</v>
       </c>
-      <c r="O9" s="71"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="94">
+      <c r="N9" s="70"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="93">
         <v>2012</v>
       </c>
-      <c r="B10" s="132">
-        <v>378330</v>
-      </c>
-      <c r="C10" s="76">
+      <c r="B10" s="75">
         <v>1835</v>
       </c>
-      <c r="D10" s="129">
+      <c r="C10" s="127">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E10" s="76">
+      <c r="D10" s="75">
         <v>33881</v>
       </c>
-      <c r="F10" s="129">
+      <c r="E10" s="127">
         <v>7.3</v>
       </c>
-      <c r="G10" s="74">
+      <c r="F10" s="73">
         <v>113949</v>
       </c>
-      <c r="H10" s="131">
+      <c r="G10" s="129">
         <v>6</v>
       </c>
-      <c r="I10" s="76">
+      <c r="H10" s="75">
         <v>143694</v>
       </c>
-      <c r="J10" s="129">
+      <c r="I10" s="127">
         <v>6.2</v>
       </c>
-      <c r="K10" s="76">
+      <c r="J10" s="75">
         <v>69481</v>
       </c>
-      <c r="L10" s="129">
+      <c r="K10" s="127">
         <v>9.9</v>
       </c>
-      <c r="M10" s="76">
+      <c r="L10" s="75">
         <v>15490</v>
       </c>
-      <c r="N10" s="133">
+      <c r="M10" s="130">
         <v>21.7</v>
       </c>
-      <c r="O10" s="71"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="94">
+      <c r="N10" s="70"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="93">
         <v>2011</v>
       </c>
-      <c r="B11" s="132">
-        <v>387840</v>
-      </c>
-      <c r="C11" s="76">
+      <c r="B11" s="75">
         <v>1809</v>
       </c>
-      <c r="D11" s="129">
+      <c r="C11" s="127">
         <v>10.9</v>
       </c>
-      <c r="E11" s="76">
+      <c r="D11" s="75">
         <v>37506</v>
       </c>
-      <c r="F11" s="129">
+      <c r="E11" s="127">
         <v>7.4</v>
       </c>
-      <c r="G11" s="74">
+      <c r="F11" s="73">
         <v>117600</v>
       </c>
-      <c r="H11" s="131">
+      <c r="G11" s="129">
         <v>6.1</v>
       </c>
-      <c r="I11" s="76">
+      <c r="H11" s="75">
         <v>144309</v>
       </c>
-      <c r="J11" s="129">
+      <c r="I11" s="127">
         <v>6.1</v>
       </c>
-      <c r="K11" s="76">
+      <c r="J11" s="75">
         <v>71218</v>
       </c>
-      <c r="L11" s="129">
+      <c r="K11" s="127">
         <v>9.8000000000000007</v>
       </c>
-      <c r="M11" s="76">
+      <c r="L11" s="75">
         <v>15398</v>
       </c>
-      <c r="N11" s="133">
+      <c r="M11" s="130">
         <v>21.1</v>
       </c>
-      <c r="O11" s="71"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="94">
+      <c r="N11" s="70"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="93">
         <v>2010</v>
       </c>
-      <c r="B12" s="132">
-        <v>390082</v>
-      </c>
-      <c r="C12" s="76">
+      <c r="B12" s="75">
         <v>2116</v>
       </c>
-      <c r="D12" s="129">
+      <c r="C12" s="127">
         <v>13.6</v>
       </c>
-      <c r="E12" s="76">
+      <c r="D12" s="75">
         <v>39702</v>
       </c>
-      <c r="F12" s="129">
+      <c r="E12" s="127">
         <v>7.5</v>
       </c>
-      <c r="G12" s="74">
+      <c r="F12" s="73">
         <v>119120</v>
       </c>
-      <c r="H12" s="131">
+      <c r="G12" s="129">
         <v>6</v>
       </c>
-      <c r="I12" s="76">
+      <c r="H12" s="75">
         <v>140813</v>
       </c>
-      <c r="J12" s="129">
+      <c r="I12" s="127">
         <v>5.9</v>
       </c>
-      <c r="K12" s="76">
+      <c r="J12" s="75">
         <v>73033</v>
       </c>
-      <c r="L12" s="129">
+      <c r="K12" s="127">
         <v>9.6</v>
       </c>
-      <c r="M12" s="76">
+      <c r="L12" s="75">
         <v>15298</v>
       </c>
-      <c r="N12" s="133">
+      <c r="M12" s="130">
         <v>21.8</v>
       </c>
-      <c r="O12" s="71"/>
-    </row>
-    <row r="13" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="94">
+      <c r="N12" s="70"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="93">
         <v>2009</v>
       </c>
-      <c r="B13" s="132">
-        <v>384552</v>
-      </c>
-      <c r="C13" s="76">
+      <c r="B13" s="75">
         <v>2878</v>
       </c>
-      <c r="D13" s="129">
+      <c r="C13" s="127">
         <v>8.6</v>
       </c>
-      <c r="E13" s="76">
+      <c r="D13" s="75">
         <v>41156</v>
       </c>
-      <c r="F13" s="129">
+      <c r="E13" s="127">
         <v>6.7</v>
       </c>
-      <c r="G13" s="76">
+      <c r="F13" s="75">
         <v>117932</v>
       </c>
-      <c r="H13" s="129">
+      <c r="G13" s="127">
         <v>5.6</v>
       </c>
-      <c r="I13" s="76">
+      <c r="H13" s="75">
         <v>136213</v>
       </c>
-      <c r="J13" s="129">
+      <c r="I13" s="127">
         <v>5.7</v>
       </c>
-      <c r="K13" s="76">
+      <c r="J13" s="75">
         <v>71823</v>
       </c>
-      <c r="L13" s="129">
+      <c r="K13" s="127">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M13" s="76">
+      <c r="L13" s="75">
         <v>14550</v>
       </c>
-      <c r="N13" s="133">
+      <c r="M13" s="130">
         <v>21.4</v>
       </c>
-      <c r="O13" s="71"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="94">
+      <c r="N13" s="70"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="93">
         <v>2008</v>
       </c>
-      <c r="B14" s="132">
-        <v>384968</v>
-      </c>
-      <c r="C14" s="76">
+      <c r="B14" s="75">
         <v>3828</v>
       </c>
-      <c r="D14" s="129">
+      <c r="C14" s="127">
         <v>8.5</v>
       </c>
-      <c r="E14" s="76">
+      <c r="D14" s="75">
         <v>42941</v>
       </c>
-      <c r="F14" s="129">
+      <c r="E14" s="127">
         <v>7</v>
       </c>
-      <c r="G14" s="76">
+      <c r="F14" s="75">
         <v>117932</v>
       </c>
-      <c r="H14" s="129">
+      <c r="G14" s="127">
         <v>6.1</v>
       </c>
-      <c r="I14" s="76">
+      <c r="H14" s="75">
         <v>133753</v>
       </c>
-      <c r="J14" s="129">
+      <c r="I14" s="127">
         <v>5.9</v>
       </c>
-      <c r="K14" s="76">
+      <c r="J14" s="75">
         <v>71891</v>
       </c>
-      <c r="L14" s="129">
+      <c r="K14" s="127">
         <v>9.8000000000000007</v>
       </c>
-      <c r="M14" s="76">
+      <c r="L14" s="75">
         <v>14623</v>
       </c>
-      <c r="N14" s="133">
+      <c r="M14" s="130">
         <v>22.3</v>
       </c>
-      <c r="O14" s="71"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="94">
+      <c r="N14" s="70"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="93">
         <v>2007</v>
       </c>
-      <c r="B15" s="132">
-        <v>391898</v>
-      </c>
-      <c r="C15" s="76">
+      <c r="B15" s="75">
         <v>4376</v>
       </c>
-      <c r="D15" s="129">
+      <c r="C15" s="127">
         <v>8.5</v>
       </c>
-      <c r="E15" s="76">
+      <c r="D15" s="75">
         <v>45094</v>
       </c>
-      <c r="F15" s="129">
+      <c r="E15" s="127">
         <v>7.1</v>
       </c>
-      <c r="G15" s="76">
+      <c r="F15" s="75">
         <v>118160</v>
       </c>
-      <c r="H15" s="129">
+      <c r="G15" s="127">
         <v>6</v>
       </c>
-      <c r="I15" s="76">
+      <c r="H15" s="75">
         <v>136823</v>
       </c>
-      <c r="J15" s="129">
+      <c r="I15" s="127">
         <v>5.8</v>
       </c>
-      <c r="K15" s="76">
+      <c r="J15" s="75">
         <v>72931</v>
       </c>
-      <c r="L15" s="129">
+      <c r="K15" s="127">
         <v>10</v>
       </c>
-      <c r="M15" s="76">
+      <c r="L15" s="75">
         <v>14514</v>
       </c>
-      <c r="N15" s="133">
+      <c r="M15" s="130">
         <v>23.9</v>
       </c>
-      <c r="O15" s="71"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="94">
+      <c r="N15" s="70"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="93">
         <v>2006</v>
       </c>
-      <c r="B16" s="132">
-        <v>383926</v>
-      </c>
-      <c r="C16" s="76">
+      <c r="B16" s="75">
         <v>4586</v>
       </c>
-      <c r="D16" s="129">
+      <c r="C16" s="127">
         <v>7.6</v>
       </c>
-      <c r="E16" s="76">
+      <c r="D16" s="75">
         <v>45029</v>
       </c>
-      <c r="F16" s="129">
+      <c r="E16" s="127">
         <v>6.5</v>
       </c>
-      <c r="G16" s="76">
+      <c r="F16" s="75">
         <v>113178</v>
       </c>
-      <c r="H16" s="129">
+      <c r="G16" s="127">
         <v>5.6</v>
       </c>
-      <c r="I16" s="76">
+      <c r="H16" s="75">
         <v>137144</v>
       </c>
-      <c r="J16" s="129">
+      <c r="I16" s="127">
         <v>5.3</v>
       </c>
-      <c r="K16" s="76">
+      <c r="J16" s="75">
         <v>70409</v>
       </c>
-      <c r="L16" s="129">
+      <c r="K16" s="127">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M16" s="76">
+      <c r="L16" s="75">
         <v>13580</v>
       </c>
-      <c r="N16" s="133">
+      <c r="M16" s="130">
         <v>22.1</v>
       </c>
-      <c r="O16" s="71"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="94">
+      <c r="N16" s="70"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="93">
         <v>2005</v>
       </c>
-      <c r="B17" s="132">
-        <v>377426</v>
-      </c>
-      <c r="C17" s="76">
+      <c r="B17" s="75">
         <v>5069</v>
       </c>
-      <c r="D17" s="129">
+      <c r="C17" s="127">
         <v>7.2</v>
       </c>
-      <c r="E17" s="76">
+      <c r="D17" s="75">
         <v>46213</v>
       </c>
-      <c r="F17" s="129">
+      <c r="E17" s="127">
         <v>7</v>
       </c>
-      <c r="G17" s="76">
+      <c r="F17" s="75">
         <v>110151</v>
       </c>
-      <c r="H17" s="129">
+      <c r="G17" s="127">
         <v>5.6</v>
       </c>
-      <c r="I17" s="76">
+      <c r="H17" s="75">
         <v>135852</v>
       </c>
-      <c r="J17" s="129">
+      <c r="I17" s="127">
         <v>5.4</v>
       </c>
-      <c r="K17" s="76">
+      <c r="J17" s="75">
         <v>67478</v>
       </c>
-      <c r="L17" s="129">
+      <c r="K17" s="127">
         <v>9.6</v>
       </c>
-      <c r="M17" s="76">
+      <c r="L17" s="75">
         <v>12663</v>
       </c>
-      <c r="N17" s="133">
+      <c r="M17" s="130">
         <v>23.1</v>
       </c>
-      <c r="O17" s="71"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="94">
+      <c r="N17" s="70"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="93">
         <v>2004</v>
       </c>
-      <c r="B18" s="132">
-        <v>372704</v>
-      </c>
-      <c r="C18" s="76">
+      <c r="B18" s="75">
         <v>5491</v>
       </c>
-      <c r="D18" s="129">
+      <c r="C18" s="127">
         <v>7</v>
       </c>
-      <c r="E18" s="76">
+      <c r="D18" s="75">
         <v>46242</v>
       </c>
-      <c r="F18" s="129">
+      <c r="E18" s="127">
         <v>6.6</v>
       </c>
-      <c r="G18" s="76">
+      <c r="F18" s="75">
         <v>107756</v>
       </c>
-      <c r="H18" s="129">
+      <c r="G18" s="127">
         <v>5.6</v>
       </c>
-      <c r="I18" s="76">
+      <c r="H18" s="75">
         <v>135958</v>
       </c>
-      <c r="J18" s="129">
+      <c r="I18" s="127">
         <v>5.4</v>
       </c>
-      <c r="K18" s="76">
+      <c r="J18" s="75">
         <v>65020</v>
       </c>
-      <c r="L18" s="129">
+      <c r="K18" s="127">
         <v>9.9</v>
       </c>
-      <c r="M18" s="76">
+      <c r="L18" s="75">
         <v>12237</v>
       </c>
-      <c r="N18" s="133">
+      <c r="M18" s="130">
         <v>23.6</v>
       </c>
-      <c r="O18" s="71"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="94">
+      <c r="N18" s="70"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="93">
         <v>2003</v>
       </c>
-      <c r="B19" s="132">
-        <v>366969</v>
-      </c>
-      <c r="C19" s="76">
+      <c r="B19" s="75">
         <v>5578</v>
       </c>
-      <c r="D19" s="129">
+      <c r="C19" s="127">
         <v>6.7</v>
       </c>
-      <c r="E19" s="76">
+      <c r="D19" s="75">
         <v>45653</v>
       </c>
-      <c r="F19" s="129">
+      <c r="E19" s="127">
         <v>6.8</v>
       </c>
-      <c r="G19" s="76">
+      <c r="F19" s="75">
         <v>106107</v>
       </c>
-      <c r="H19" s="129">
+      <c r="G19" s="127">
         <v>5.5</v>
       </c>
-      <c r="I19" s="76">
+      <c r="H19" s="75">
         <v>135251</v>
       </c>
-      <c r="J19" s="129">
+      <c r="I19" s="127">
         <v>5.6</v>
       </c>
-      <c r="K19" s="76">
+      <c r="J19" s="75">
         <v>62925</v>
       </c>
-      <c r="L19" s="129">
+      <c r="K19" s="127">
         <v>10.6</v>
       </c>
-      <c r="M19" s="76">
+      <c r="L19" s="75">
         <v>11455</v>
       </c>
-      <c r="N19" s="133">
+      <c r="M19" s="130">
         <v>25.8</v>
       </c>
-      <c r="O19" s="71"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="94">
+      <c r="N19" s="70"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="93">
         <v>2002</v>
       </c>
-      <c r="B20" s="132">
-        <v>365714</v>
-      </c>
-      <c r="C20" s="76">
+      <c r="B20" s="75">
         <v>6088</v>
       </c>
-      <c r="D20" s="129">
+      <c r="C20" s="127">
         <v>7</v>
       </c>
-      <c r="E20" s="76">
+      <c r="D20" s="75">
         <v>45417</v>
       </c>
-      <c r="F20" s="129">
+      <c r="E20" s="127">
         <v>7.1</v>
       </c>
-      <c r="G20" s="76">
+      <c r="F20" s="75">
         <v>108144</v>
       </c>
-      <c r="H20" s="129">
+      <c r="G20" s="127">
         <v>5.8</v>
       </c>
-      <c r="I20" s="76">
+      <c r="H20" s="75">
         <v>133619</v>
       </c>
-      <c r="J20" s="129">
+      <c r="I20" s="127">
         <v>6.3</v>
       </c>
-      <c r="K20" s="76">
+      <c r="J20" s="75">
         <v>61434</v>
       </c>
-      <c r="L20" s="129">
+      <c r="K20" s="127">
         <v>11.9</v>
       </c>
-      <c r="M20" s="76">
+      <c r="L20" s="75">
         <v>11012</v>
       </c>
-      <c r="N20" s="133">
+      <c r="M20" s="130">
         <v>27.2</v>
       </c>
-      <c r="O20" s="71"/>
-    </row>
-    <row r="21" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="94">
+      <c r="N20" s="70"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="93">
         <v>2001</v>
       </c>
-      <c r="B21" s="132">
-        <v>359245</v>
-      </c>
-      <c r="C21" s="76">
+      <c r="B21" s="75">
         <v>6267</v>
       </c>
-      <c r="D21" s="129">
+      <c r="C21" s="127">
         <v>6</v>
       </c>
-      <c r="E21" s="76">
+      <c r="D21" s="75">
         <v>45069</v>
       </c>
-      <c r="F21" s="129">
+      <c r="E21" s="127">
         <v>7.3</v>
       </c>
-      <c r="G21" s="76">
+      <c r="F21" s="75">
         <v>108920</v>
       </c>
-      <c r="H21" s="129">
+      <c r="G21" s="127">
         <v>6.3</v>
       </c>
-      <c r="I21" s="76">
+      <c r="H21" s="75">
         <v>130136</v>
       </c>
-      <c r="J21" s="129">
+      <c r="I21" s="127">
         <v>7.2</v>
       </c>
-      <c r="K21" s="76">
+      <c r="J21" s="75">
         <v>58391</v>
       </c>
-      <c r="L21" s="129">
+      <c r="K21" s="127">
         <v>13.7</v>
       </c>
-      <c r="M21" s="76">
+      <c r="L21" s="75">
         <v>10462</v>
       </c>
-      <c r="N21" s="133">
+      <c r="M21" s="130">
         <v>29</v>
       </c>
-      <c r="O21" s="71"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="94">
+      <c r="N21" s="70"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="93">
         <v>2000</v>
       </c>
-      <c r="B22" s="132">
-        <v>366196</v>
-      </c>
-      <c r="C22" s="76">
+      <c r="B22" s="75">
         <v>6486</v>
       </c>
-      <c r="D22" s="129">
+      <c r="C22" s="127">
         <v>6.8</v>
       </c>
-      <c r="E22" s="76">
+      <c r="D22" s="75">
         <v>45048</v>
       </c>
-      <c r="F22" s="129">
+      <c r="E22" s="127">
         <v>7.2</v>
       </c>
-      <c r="G22" s="76">
+      <c r="F22" s="75">
         <v>116917</v>
       </c>
-      <c r="H22" s="129">
+      <c r="G22" s="127">
         <v>6.1</v>
       </c>
-      <c r="I22" s="76">
+      <c r="H22" s="75">
         <v>130441</v>
       </c>
-      <c r="J22" s="129">
+      <c r="I22" s="127">
         <v>7.2</v>
       </c>
-      <c r="K22" s="76">
+      <c r="J22" s="75">
         <v>56990</v>
       </c>
-      <c r="L22" s="129">
+      <c r="K22" s="127">
         <v>13.8</v>
       </c>
-      <c r="M22" s="76">
+      <c r="L22" s="75">
         <v>10314</v>
       </c>
-      <c r="N22" s="133">
+      <c r="M22" s="130">
         <v>30.3</v>
       </c>
-      <c r="O22" s="71"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="94">
+      <c r="N22" s="70"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="93">
         <v>1999</v>
       </c>
-      <c r="B23" s="128">
-        <v>373520</v>
-      </c>
-      <c r="C23" s="74">
+      <c r="B23" s="73">
         <v>6437</v>
       </c>
-      <c r="D23" s="131">
+      <c r="C23" s="129">
         <v>7</v>
       </c>
-      <c r="E23" s="74">
+      <c r="D23" s="73">
         <v>45597</v>
       </c>
-      <c r="F23" s="131">
+      <c r="E23" s="129">
         <v>6.9</v>
       </c>
-      <c r="G23" s="74">
+      <c r="F23" s="73">
         <v>123533</v>
       </c>
-      <c r="H23" s="131">
+      <c r="G23" s="129">
         <v>6</v>
       </c>
-      <c r="I23" s="74">
+      <c r="H23" s="73">
         <v>132438</v>
       </c>
-      <c r="J23" s="131">
+      <c r="I23" s="129">
         <v>7.7</v>
       </c>
-      <c r="K23" s="74">
+      <c r="J23" s="73">
         <v>55804</v>
       </c>
-      <c r="L23" s="131">
+      <c r="K23" s="129">
         <v>14.8</v>
       </c>
-      <c r="M23" s="74">
+      <c r="L23" s="73">
         <v>9711</v>
       </c>
-      <c r="N23" s="130">
+      <c r="M23" s="128">
         <v>32.5</v>
       </c>
-      <c r="O23" s="71"/>
-    </row>
-    <row r="24" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="134">
+      <c r="N23" s="70"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="131">
         <v>1998</v>
       </c>
-      <c r="B24" s="135">
-        <v>388823</v>
+      <c r="B24" s="79">
+        <v>6737</v>
       </c>
       <c r="C24" s="80">
-        <v>6737</v>
-      </c>
-      <c r="D24" s="81">
         <v>6.8</v>
       </c>
+      <c r="D24" s="79">
+        <v>48892</v>
+      </c>
       <c r="E24" s="80">
-        <v>48892</v>
-      </c>
-      <c r="F24" s="81">
         <v>6.6</v>
       </c>
+      <c r="F24" s="79">
+        <v>133225</v>
+      </c>
       <c r="G24" s="80">
-        <v>133225</v>
-      </c>
-      <c r="H24" s="81">
         <v>6</v>
       </c>
+      <c r="H24" s="79">
+        <v>136324</v>
+      </c>
       <c r="I24" s="80">
-        <v>136324</v>
-      </c>
-      <c r="J24" s="81">
         <v>8.1</v>
       </c>
+      <c r="J24" s="79">
+        <v>54127</v>
+      </c>
       <c r="K24" s="80">
-        <v>54127</v>
-      </c>
-      <c r="L24" s="81">
         <v>15.3</v>
       </c>
-      <c r="M24" s="80">
+      <c r="L24" s="79">
         <v>9518</v>
       </c>
-      <c r="N24" s="136">
+      <c r="M24" s="132">
         <v>33.700000000000003</v>
       </c>
-      <c r="O24" s="71"/>
-    </row>
-    <row r="25" spans="1:15" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="82"/>
-      <c r="B25" s="69"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="70"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="81"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-    </row>
-    <row r="27" spans="1:15" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="82"/>
-      <c r="B27" s="69"/>
-    </row>
-    <row r="28" spans="1:15" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="82"/>
-      <c r="B28" s="69"/>
-    </row>
-    <row r="29" spans="1:15" s="84" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="83"/>
-    </row>
-    <row r="30" spans="1:15" ht="13" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
-    </row>
-    <row r="31" spans="1:15" ht="13" x14ac:dyDescent="0.3">
-      <c r="B31" s="69"/>
-    </row>
-    <row r="32" spans="1:15" ht="13" x14ac:dyDescent="0.3">
-      <c r="B32" s="69"/>
-    </row>
-    <row r="33" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="B33" s="69"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="85"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="81"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="81"/>
+    </row>
+    <row r="29" spans="1:14" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="82"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="84"/>
       <c r="B34" s="86"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
-      <c r="B35" s="86"/>
-    </row>
-    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="82"/>
-      <c r="B36" s="88"/>
-    </row>
-    <row r="37" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="B37" s="88"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="81"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11214,217 +11097,219 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0184AA3D-B92E-4425-9BBD-A7B70C976138}">
   <dimension ref="A1:AX25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AX1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.61328125" style="70" customWidth="1"/>
-    <col min="2" max="24" width="17.4609375" style="70" customWidth="1"/>
-    <col min="25" max="16384" width="9.07421875" style="70"/>
+    <col min="1" max="1" width="15.61328125" style="69" customWidth="1"/>
+    <col min="2" max="2" width="17.4609375" style="69" customWidth="1"/>
+    <col min="3" max="3" width="17.4609375" style="83" customWidth="1"/>
+    <col min="4" max="24" width="17.4609375" style="69" customWidth="1"/>
+    <col min="25" max="16384" width="9.07421875" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="100" t="s">
+      <c r="B1" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="C1" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="D1" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="101" t="s">
+      <c r="E1" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="F1" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="G1" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="H1" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="101" t="s">
+      <c r="I1" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="100" t="s">
+      <c r="J1" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="101" t="s">
+      <c r="K1" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="100" t="s">
+      <c r="L1" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="101" t="s">
+      <c r="M1" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="100" t="s">
+      <c r="N1" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="102" t="s">
+      <c r="O1" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="100" t="s">
+      <c r="P1" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="101" t="s">
+      <c r="Q1" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="100" t="s">
+      <c r="R1" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="102" t="s">
+      <c r="S1" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="100" t="s">
+      <c r="T1" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="101" t="s">
+      <c r="U1" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="100" t="s">
+      <c r="V1" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="99" t="s">
+      <c r="W1" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" s="70" t="str">
+      <c r="X1" s="98" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Year of conception]])</f>
         <v>Year of conception</v>
       </c>
-      <c r="AB1" s="70" t="str">
+      <c r="AB1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age under 20
 Number of conceptions]])</f>
         <v>Age under 20Number of conceptions</v>
       </c>
-      <c r="AC1" s="70" t="str">
+      <c r="AC1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age under 20
 Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership]])</f>
         <v>Age under 20Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership</v>
       </c>
-      <c r="AD1" s="70" t="str">
+      <c r="AD1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age under 20
 Percentage of conceptions leading to abortion]])</f>
         <v>Age under 20Percentage of conceptions leading to abortion</v>
       </c>
-      <c r="AE1" s="70" t="str">
+      <c r="AE1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 20 to 24
 Percentage of conceptions outside marriage or civil partnership ]])</f>
         <v xml:space="preserve">Age 20 to 24Percentage of conceptions outside marriage or civil partnership </v>
       </c>
-      <c r="AF1" s="70" t="str">
+      <c r="AF1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 20 to 24
 Number of conceptions]])</f>
         <v>Age 20 to 24Number of conceptions</v>
       </c>
-      <c r="AG1" s="70" t="str">
+      <c r="AG1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 20 to 24
 Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership]])</f>
         <v>Age 20 to 24Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership</v>
       </c>
-      <c r="AH1" s="70" t="str">
+      <c r="AH1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 20 to 24
 Percentage of conceptions leading to abortion]])</f>
         <v>Age 20 to 24Percentage of conceptions leading to abortion</v>
       </c>
-      <c r="AI1" s="70" t="str">
+      <c r="AI1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 25 to 29
 Percentage of conceptions outside marriage or civil partnership]])</f>
         <v>Age 25 to 29Percentage of conceptions outside marriage or civil partnership</v>
       </c>
-      <c r="AJ1" s="70" t="str">
+      <c r="AJ1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 25 to 29
 Number of conceptions]])</f>
         <v>Age 25 to 29Number of conceptions</v>
       </c>
-      <c r="AK1" s="70" t="str">
+      <c r="AK1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 25 to 29
 Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership]])</f>
         <v>Age 25 to 29Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership</v>
       </c>
-      <c r="AL1" s="70" t="str">
+      <c r="AL1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 25 to 29
 Percentage of conceptions leading to abortion]])</f>
         <v>Age 25 to 29Percentage of conceptions leading to abortion</v>
       </c>
-      <c r="AM1" s="70" t="str">
+      <c r="AM1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 30 to 34
 Percentage of conceptions outside marriage or civil partnership]])</f>
         <v>Age 30 to 34Percentage of conceptions outside marriage or civil partnership</v>
       </c>
-      <c r="AN1" s="70" t="str">
+      <c r="AN1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 30 to 34
 Number of conceptions]])</f>
         <v>Age 30 to 34Number of conceptions</v>
       </c>
-      <c r="AO1" s="70" t="str">
+      <c r="AO1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 30 to 34
 Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership]])</f>
         <v>Age 30 to 34Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership</v>
       </c>
-      <c r="AP1" s="70" t="str">
+      <c r="AP1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 30 to 34
 Percentage of conceptions leading to abortion]])</f>
         <v>Age 30 to 34Percentage of conceptions leading to abortion</v>
       </c>
-      <c r="AQ1" s="70" t="str">
+      <c r="AQ1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 35 to 39
 Percentage of conceptions outside marriage or civil partnership ]])</f>
         <v xml:space="preserve">Age 35 to 39Percentage of conceptions outside marriage or civil partnership </v>
       </c>
-      <c r="AR1" s="70" t="str">
+      <c r="AR1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 35 to 39
 Number of conceptions]])</f>
         <v>Age 35 to 39Number of conceptions</v>
       </c>
-      <c r="AS1" s="70" t="str">
+      <c r="AS1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 35 to 39
 Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership ]])</f>
         <v xml:space="preserve">Age 35 to 39Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership </v>
       </c>
-      <c r="AT1" s="70" t="str">
+      <c r="AT1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 35 to 39 Percentage of conceptions leading to abortion]])</f>
         <v>Age 35 to 39 Percentage of conceptions leading to abortion</v>
       </c>
-      <c r="AU1" s="70" t="str">
+      <c r="AU1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 40 and over
 Percentage of conceptions outside marriage or civil partnership]])</f>
         <v>Age 40 and overPercentage of conceptions outside marriage or civil partnership</v>
       </c>
-      <c r="AV1" s="70" t="str">
+      <c r="AV1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 40 and over
 Number of conceptions]])</f>
         <v>Age 40 and overNumber of conceptions</v>
       </c>
-      <c r="AW1" s="70" t="str">
+      <c r="AW1" s="69" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 40 and over
 Percentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership]])</f>
         <v>Age 40 and overPercentage of conceptions outside marriage or civil partnership leading to a maternity within marriage or civil partnership</v>
       </c>
-      <c r="AX1" s="86" t="str">
+      <c r="AX1" s="85" t="str">
         <f>CLEAN(Table311[[#Headers],[Age 40 and over
 Percentage of conceptions leading to abortion]])</f>
         <v>Age 40 and overPercentage of conceptions leading to abortion</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="93">
+      <c r="A2" s="92">
         <v>2020</v>
       </c>
       <c r="B2" s="19">
         <v>4916</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="134">
         <v>0.5</v>
       </c>
       <c r="D2" s="18">
@@ -11492,13 +11377,13 @@
       </c>
     </row>
     <row r="3" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="93">
+      <c r="A3" s="92">
         <v>2019</v>
       </c>
       <c r="B3" s="19">
         <v>47118</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="134">
         <v>0.7</v>
       </c>
       <c r="D3" s="24">
@@ -11552,7 +11437,7 @@
       <c r="T3" s="23">
         <v>30.3</v>
       </c>
-      <c r="U3" s="72">
+      <c r="U3" s="71">
         <v>48.5</v>
       </c>
       <c r="V3" s="19">
@@ -11566,1561 +11451,1561 @@
       </c>
     </row>
     <row r="4" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="93">
+      <c r="A4" s="92">
         <v>2018</v>
       </c>
-      <c r="B4" s="74">
+      <c r="B4" s="73">
         <v>49657</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="135">
         <v>0.8</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="94">
         <v>49.5</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="70">
         <v>85.8</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="73">
         <v>130070</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="78">
         <v>2</v>
       </c>
-      <c r="H4" s="95">
+      <c r="H4" s="94">
         <v>39.5</v>
       </c>
-      <c r="I4" s="71">
+      <c r="I4" s="70">
         <v>61.8</v>
       </c>
-      <c r="J4" s="74">
+      <c r="J4" s="73">
         <v>145492</v>
       </c>
-      <c r="K4" s="71">
+      <c r="K4" s="70">
         <v>3.3</v>
       </c>
-      <c r="L4" s="96">
+      <c r="L4" s="95">
         <v>30.5</v>
       </c>
-      <c r="M4" s="71">
+      <c r="M4" s="70">
         <v>42.8</v>
       </c>
-      <c r="N4" s="74">
+      <c r="N4" s="73">
         <v>93728</v>
       </c>
-      <c r="O4" s="71">
+      <c r="O4" s="70">
         <v>3.5</v>
       </c>
-      <c r="P4" s="95">
+      <c r="P4" s="94">
         <v>27.8</v>
       </c>
-      <c r="Q4" s="71">
+      <c r="Q4" s="70">
         <v>42.3</v>
       </c>
-      <c r="R4" s="74">
+      <c r="R4" s="73">
         <v>54854</v>
       </c>
-      <c r="S4" s="71">
+      <c r="S4" s="70">
         <v>3.5</v>
       </c>
-      <c r="T4" s="95">
+      <c r="T4" s="94">
         <v>28.5</v>
       </c>
-      <c r="U4" s="73">
+      <c r="U4" s="72">
         <v>48.3</v>
       </c>
-      <c r="V4" s="74">
+      <c r="V4" s="73">
         <v>1496</v>
       </c>
-      <c r="W4" s="71">
+      <c r="W4" s="70">
         <v>2.8</v>
       </c>
-      <c r="X4" s="71">
+      <c r="X4" s="70">
         <v>36.6</v>
       </c>
     </row>
     <row r="5" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="93">
+      <c r="A5" s="92">
         <v>2017</v>
       </c>
-      <c r="B5" s="74">
+      <c r="B5" s="73">
         <v>51538</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="135">
         <v>0.9</v>
       </c>
-      <c r="D5" s="96">
+      <c r="D5" s="95">
         <v>48</v>
       </c>
-      <c r="E5" s="71">
+      <c r="E5" s="70">
         <v>85.9</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="73">
         <v>133501</v>
       </c>
-      <c r="G5" s="71">
+      <c r="G5" s="70">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H5" s="95">
+      <c r="H5" s="94">
         <v>37.5</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5" s="70">
         <v>60.3</v>
       </c>
-      <c r="J5" s="74">
+      <c r="J5" s="73">
         <v>145025</v>
       </c>
-      <c r="K5" s="71">
+      <c r="K5" s="70">
         <v>3.6</v>
       </c>
-      <c r="L5" s="96">
+      <c r="L5" s="95">
         <v>29</v>
       </c>
-      <c r="M5" s="71">
+      <c r="M5" s="70">
         <v>41.6</v>
       </c>
-      <c r="N5" s="74">
+      <c r="N5" s="73">
         <v>90098</v>
       </c>
-      <c r="O5" s="71">
+      <c r="O5" s="70">
         <v>3.9</v>
       </c>
-      <c r="P5" s="95">
+      <c r="P5" s="94">
         <v>25.9</v>
       </c>
-      <c r="Q5" s="71">
+      <c r="Q5" s="70">
         <v>41.4</v>
       </c>
-      <c r="R5" s="74">
+      <c r="R5" s="73">
         <v>53215</v>
       </c>
-      <c r="S5" s="71">
+      <c r="S5" s="70">
         <v>3.7</v>
       </c>
-      <c r="T5" s="95">
+      <c r="T5" s="94">
         <v>27.2</v>
       </c>
-      <c r="U5" s="73">
+      <c r="U5" s="72">
         <v>47.3</v>
       </c>
-      <c r="V5" s="74">
+      <c r="V5" s="73">
         <v>13629</v>
       </c>
-      <c r="W5" s="79">
+      <c r="W5" s="78">
         <v>3</v>
       </c>
-      <c r="X5" s="71">
+      <c r="X5" s="70">
         <v>35.200000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="93">
+      <c r="A6" s="92">
         <v>2016</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="75">
         <v>54577</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="136">
         <v>0.8</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="76">
         <v>46.7</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="77">
         <v>85.2</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="75">
         <v>137470</v>
       </c>
-      <c r="G6" s="77">
+      <c r="G6" s="76">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="76">
         <v>35.9</v>
       </c>
-      <c r="I6" s="78">
+      <c r="I6" s="77">
         <v>58.5</v>
       </c>
-      <c r="J6" s="76">
+      <c r="J6" s="75">
         <v>144580</v>
       </c>
-      <c r="K6" s="77">
+      <c r="K6" s="76">
         <v>3.7</v>
       </c>
-      <c r="L6" s="77">
+      <c r="L6" s="76">
         <v>28.1</v>
       </c>
-      <c r="M6" s="90">
+      <c r="M6" s="89">
         <v>40.200000000000003</v>
       </c>
-      <c r="N6" s="76">
+      <c r="N6" s="75">
         <v>97451</v>
       </c>
-      <c r="O6" s="89">
+      <c r="O6" s="88">
         <v>4.3</v>
       </c>
-      <c r="P6" s="89">
+      <c r="P6" s="88">
         <v>25.2</v>
       </c>
-      <c r="Q6" s="90">
+      <c r="Q6" s="89">
         <v>40.4</v>
       </c>
-      <c r="R6" s="76">
+      <c r="R6" s="75">
         <v>51300</v>
       </c>
-      <c r="S6" s="89">
+      <c r="S6" s="88">
         <v>4</v>
       </c>
-      <c r="T6" s="89">
+      <c r="T6" s="88">
         <v>26.7</v>
       </c>
-      <c r="U6" s="90">
+      <c r="U6" s="89">
         <v>46.6</v>
       </c>
-      <c r="V6" s="76">
+      <c r="V6" s="75">
         <v>13389</v>
       </c>
-      <c r="W6" s="89">
+      <c r="W6" s="88">
         <v>3.3</v>
       </c>
-      <c r="X6" s="89">
+      <c r="X6" s="88">
         <v>35.4</v>
       </c>
     </row>
     <row r="7" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="93">
+      <c r="A7" s="92">
         <v>2015</v>
       </c>
-      <c r="B7" s="74">
+      <c r="B7" s="73">
         <v>58182</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="135">
         <v>0.9</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="70">
         <v>46.3</v>
       </c>
-      <c r="E7" s="73">
+      <c r="E7" s="72">
         <v>84.8</v>
       </c>
-      <c r="F7" s="74">
+      <c r="F7" s="73">
         <v>142865</v>
       </c>
-      <c r="G7" s="71">
+      <c r="G7" s="70">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="70">
         <v>34.700000000000003</v>
       </c>
-      <c r="I7" s="73">
+      <c r="I7" s="72">
         <v>56.7</v>
       </c>
-      <c r="J7" s="74">
+      <c r="J7" s="73">
         <v>141840</v>
       </c>
-      <c r="K7" s="71">
+      <c r="K7" s="70">
         <v>3.9</v>
       </c>
-      <c r="L7" s="71">
+      <c r="L7" s="70">
         <v>27.3</v>
       </c>
-      <c r="M7" s="73">
+      <c r="M7" s="72">
         <v>39.5</v>
       </c>
-      <c r="N7" s="74">
+      <c r="N7" s="73">
         <v>96683</v>
       </c>
-      <c r="O7" s="71">
+      <c r="O7" s="70">
         <v>4.3</v>
       </c>
-      <c r="P7" s="71">
+      <c r="P7" s="70">
         <v>24.7</v>
       </c>
-      <c r="Q7" s="73">
+      <c r="Q7" s="72">
         <v>39.700000000000003</v>
       </c>
-      <c r="R7" s="74">
+      <c r="R7" s="73">
         <v>49489</v>
       </c>
-      <c r="S7" s="71">
+      <c r="S7" s="70">
         <v>4.0999999999999996</v>
       </c>
-      <c r="T7" s="71">
+      <c r="T7" s="70">
         <v>25.9</v>
       </c>
-      <c r="U7" s="73">
+      <c r="U7" s="72">
         <v>46.3</v>
       </c>
-      <c r="V7" s="74">
+      <c r="V7" s="73">
         <v>13529</v>
       </c>
-      <c r="W7" s="71">
+      <c r="W7" s="70">
         <v>3.5</v>
       </c>
-      <c r="X7" s="71">
+      <c r="X7" s="70">
         <v>35.1</v>
       </c>
     </row>
     <row r="8" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="93">
+      <c r="A8" s="92">
         <v>2014</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="75">
         <v>61429</v>
       </c>
-      <c r="C8" s="77">
+      <c r="C8" s="136">
         <v>0.9</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="76">
         <v>45.5</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E8" s="77">
         <v>84.4</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="75">
         <v>146771</v>
       </c>
-      <c r="G8" s="77">
+      <c r="G8" s="76">
         <v>2.4</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="76">
         <v>34.200000000000003</v>
       </c>
-      <c r="I8" s="78">
+      <c r="I8" s="77">
         <v>55.6</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="75">
         <v>137539</v>
       </c>
-      <c r="K8" s="77">
+      <c r="K8" s="76">
         <v>3.9</v>
       </c>
-      <c r="L8" s="77">
+      <c r="L8" s="76">
         <v>27</v>
       </c>
-      <c r="M8" s="90">
+      <c r="M8" s="89">
         <v>39</v>
       </c>
-      <c r="N8" s="76">
+      <c r="N8" s="75">
         <v>93661</v>
       </c>
-      <c r="O8" s="89">
+      <c r="O8" s="88">
         <v>4.5</v>
       </c>
-      <c r="P8" s="89">
+      <c r="P8" s="88">
         <v>24.1</v>
       </c>
-      <c r="Q8" s="90">
+      <c r="Q8" s="89">
         <v>39.700000000000003</v>
       </c>
-      <c r="R8" s="76">
+      <c r="R8" s="75">
         <v>46812</v>
       </c>
-      <c r="S8" s="89">
+      <c r="S8" s="88">
         <v>4.2</v>
       </c>
-      <c r="T8" s="89">
+      <c r="T8" s="88">
         <v>25.8</v>
       </c>
-      <c r="U8" s="90">
+      <c r="U8" s="89">
         <v>46.5</v>
       </c>
-      <c r="V8" s="76">
+      <c r="V8" s="75">
         <v>13315</v>
       </c>
-      <c r="W8" s="89">
+      <c r="W8" s="88">
         <v>3.6</v>
       </c>
-      <c r="X8" s="89">
+      <c r="X8" s="88">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="93">
+      <c r="A9" s="92">
         <v>2013</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="75">
         <v>66117</v>
       </c>
-      <c r="C9" s="77">
+      <c r="C9" s="136">
         <v>0.9</v>
       </c>
-      <c r="D9" s="77">
+      <c r="D9" s="76">
         <v>45.1</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="72">
         <v>83.5</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="75">
         <v>150716</v>
       </c>
-      <c r="G9" s="77">
+      <c r="G9" s="76">
         <v>2.5</v>
       </c>
-      <c r="H9" s="77">
+      <c r="H9" s="76">
         <v>34.299999999999997</v>
       </c>
-      <c r="I9" s="78">
+      <c r="I9" s="77">
         <v>54.4</v>
       </c>
-      <c r="J9" s="74">
+      <c r="J9" s="73">
         <v>133616</v>
       </c>
-      <c r="K9" s="79">
+      <c r="K9" s="78">
         <v>4</v>
       </c>
-      <c r="L9" s="79">
+      <c r="L9" s="78">
         <v>27.2</v>
       </c>
-      <c r="M9" s="90">
+      <c r="M9" s="89">
         <v>38.6</v>
       </c>
-      <c r="N9" s="76">
+      <c r="N9" s="75">
         <v>90997</v>
       </c>
-      <c r="O9" s="89">
+      <c r="O9" s="88">
         <v>4.5</v>
       </c>
-      <c r="P9" s="89">
+      <c r="P9" s="88">
         <v>24.2</v>
       </c>
-      <c r="Q9" s="90">
+      <c r="Q9" s="89">
         <v>39.200000000000003</v>
       </c>
-      <c r="R9" s="76">
+      <c r="R9" s="75">
         <v>44794</v>
       </c>
-      <c r="S9" s="89">
+      <c r="S9" s="88">
         <v>4.2</v>
       </c>
-      <c r="T9" s="89">
+      <c r="T9" s="88">
         <v>25.6</v>
       </c>
-      <c r="U9" s="90">
+      <c r="U9" s="89">
         <v>46.2</v>
       </c>
-      <c r="V9" s="76">
+      <c r="V9" s="75">
         <v>13238</v>
       </c>
-      <c r="W9" s="89">
+      <c r="W9" s="88">
         <v>3.6</v>
       </c>
-      <c r="X9" s="89">
+      <c r="X9" s="88">
         <v>35.5</v>
       </c>
     </row>
     <row r="10" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="93">
+      <c r="A10" s="92">
         <v>2012</v>
       </c>
-      <c r="B10" s="76">
+      <c r="B10" s="75">
         <v>73113</v>
       </c>
-      <c r="C10" s="77">
+      <c r="C10" s="136">
         <v>0.9</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="76">
         <v>43.9</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="77">
         <v>82.2</v>
       </c>
-      <c r="F10" s="76">
+      <c r="F10" s="75">
         <v>15691</v>
       </c>
-      <c r="G10" s="77">
+      <c r="G10" s="76">
         <v>2.6</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="76">
         <v>33.200000000000003</v>
       </c>
-      <c r="I10" s="78">
+      <c r="I10" s="77">
         <v>53.5</v>
       </c>
-      <c r="J10" s="74">
+      <c r="J10" s="73">
         <v>131233</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="78">
         <v>4.7</v>
       </c>
-      <c r="L10" s="79">
+      <c r="L10" s="78">
         <v>26.4</v>
       </c>
-      <c r="M10" s="90">
+      <c r="M10" s="89">
         <v>38</v>
       </c>
-      <c r="N10" s="76">
+      <c r="N10" s="75">
         <v>87929</v>
       </c>
-      <c r="O10" s="89">
+      <c r="O10" s="88">
         <v>5</v>
       </c>
-      <c r="P10" s="89">
+      <c r="P10" s="88">
         <v>24.1</v>
       </c>
-      <c r="Q10" s="90">
+      <c r="Q10" s="89">
         <v>39.200000000000003</v>
       </c>
-      <c r="R10" s="76">
+      <c r="R10" s="75">
         <v>44818</v>
       </c>
-      <c r="S10" s="89">
+      <c r="S10" s="88">
         <v>4.5999999999999996</v>
       </c>
-      <c r="T10" s="89">
+      <c r="T10" s="88">
         <v>25.4</v>
       </c>
-      <c r="U10" s="90">
+      <c r="U10" s="89">
         <v>46.1</v>
       </c>
-      <c r="V10" s="76">
+      <c r="V10" s="75">
         <v>13224</v>
       </c>
-      <c r="W10" s="89">
+      <c r="W10" s="88">
         <v>3.9</v>
       </c>
-      <c r="X10" s="89">
+      <c r="X10" s="88">
         <v>35.5</v>
       </c>
     </row>
     <row r="11" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="93">
+      <c r="A11" s="92">
         <v>2011</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="75">
         <v>82206</v>
       </c>
-      <c r="C11" s="77">
+      <c r="C11" s="136">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="76">
         <v>43.2</v>
       </c>
-      <c r="E11" s="73">
+      <c r="E11" s="72">
         <v>81.2</v>
       </c>
-      <c r="F11" s="76">
+      <c r="F11" s="75">
         <v>162385</v>
       </c>
-      <c r="G11" s="77">
+      <c r="G11" s="76">
         <v>2.8</v>
       </c>
-      <c r="H11" s="77">
+      <c r="H11" s="76">
         <v>32.4</v>
       </c>
-      <c r="I11" s="78">
+      <c r="I11" s="77">
         <v>52.7</v>
       </c>
-      <c r="J11" s="74">
+      <c r="J11" s="73">
         <v>13963</v>
       </c>
-      <c r="K11" s="79">
+      <c r="K11" s="78">
         <v>4.7</v>
       </c>
-      <c r="L11" s="79">
+      <c r="L11" s="78">
         <v>26.6</v>
       </c>
-      <c r="M11" s="90">
+      <c r="M11" s="89">
         <v>37.6</v>
       </c>
-      <c r="N11" s="76">
+      <c r="N11" s="75">
         <v>86840</v>
       </c>
-      <c r="O11" s="89">
+      <c r="O11" s="88">
         <v>5.0999999999999996</v>
       </c>
-      <c r="P11" s="89">
+      <c r="P11" s="88">
         <v>23.8</v>
       </c>
-      <c r="Q11" s="90">
+      <c r="Q11" s="89">
         <v>38.9</v>
       </c>
-      <c r="R11" s="76">
+      <c r="R11" s="75">
         <v>45426</v>
       </c>
-      <c r="S11" s="89">
+      <c r="S11" s="88">
         <v>4.5999999999999996</v>
       </c>
-      <c r="T11" s="89">
+      <c r="T11" s="88">
         <v>25.7</v>
       </c>
-      <c r="U11" s="90">
+      <c r="U11" s="89">
         <v>46.4</v>
       </c>
-      <c r="V11" s="76">
+      <c r="V11" s="75">
         <v>13349</v>
       </c>
-      <c r="W11" s="89">
+      <c r="W11" s="88">
         <v>3.9</v>
       </c>
-      <c r="X11" s="89">
+      <c r="X11" s="88">
         <v>35.799999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="93">
+      <c r="A12" s="92">
         <v>2010</v>
       </c>
-      <c r="B12" s="76">
+      <c r="B12" s="75">
         <v>89563</v>
       </c>
-      <c r="C12" s="89">
+      <c r="C12" s="137">
         <v>1</v>
       </c>
-      <c r="D12" s="89">
+      <c r="D12" s="88">
         <v>43.5</v>
       </c>
-      <c r="E12" s="92">
+      <c r="E12" s="91">
         <v>80.3</v>
       </c>
-      <c r="F12" s="74">
+      <c r="F12" s="73">
         <v>161873</v>
       </c>
-      <c r="G12" s="91">
+      <c r="G12" s="90">
         <v>3</v>
       </c>
-      <c r="H12" s="91">
+      <c r="H12" s="90">
         <v>32.200000000000003</v>
       </c>
-      <c r="I12" s="90">
+      <c r="I12" s="89">
         <v>51.8</v>
       </c>
-      <c r="J12" s="76">
+      <c r="J12" s="75">
         <v>128218</v>
       </c>
-      <c r="K12" s="89">
+      <c r="K12" s="88">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L12" s="89">
+      <c r="L12" s="88">
         <v>26</v>
       </c>
-      <c r="M12" s="90">
+      <c r="M12" s="89">
         <v>36.700000000000003</v>
       </c>
-      <c r="N12" s="76">
+      <c r="N12" s="75">
         <v>81595</v>
       </c>
-      <c r="O12" s="89">
+      <c r="O12" s="88">
         <v>5.5</v>
       </c>
-      <c r="P12" s="89">
+      <c r="P12" s="88">
         <v>24</v>
       </c>
-      <c r="Q12" s="90">
+      <c r="Q12" s="89">
         <v>38.299999999999997</v>
       </c>
-      <c r="R12" s="76">
+      <c r="R12" s="75">
         <v>45293</v>
       </c>
-      <c r="S12" s="89">
+      <c r="S12" s="88">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T12" s="89">
+      <c r="T12" s="88">
         <v>26.1</v>
       </c>
-      <c r="U12" s="90">
+      <c r="U12" s="89">
         <v>45.2</v>
       </c>
-      <c r="V12" s="76">
+      <c r="V12" s="75">
         <v>12621</v>
       </c>
-      <c r="W12" s="89">
+      <c r="W12" s="88">
         <v>3.9</v>
       </c>
-      <c r="X12" s="89">
+      <c r="X12" s="88">
         <v>36.1</v>
       </c>
     </row>
     <row r="13" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="94">
+      <c r="A13" s="93">
         <v>2009</v>
       </c>
-      <c r="B13" s="76">
+      <c r="B13" s="75">
         <v>95063</v>
       </c>
-      <c r="C13" s="89">
+      <c r="C13" s="137">
         <v>1</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="88">
         <v>42.9</v>
       </c>
-      <c r="E13" s="92">
+      <c r="E13" s="91">
         <v>79.400000000000006</v>
       </c>
-      <c r="F13" s="74">
+      <c r="F13" s="73">
         <v>158380</v>
       </c>
-      <c r="G13" s="91">
+      <c r="G13" s="90">
         <v>3</v>
       </c>
-      <c r="H13" s="91">
+      <c r="H13" s="90">
         <v>32.4</v>
       </c>
-      <c r="I13" s="90">
+      <c r="I13" s="89">
         <v>51.3</v>
       </c>
-      <c r="J13" s="76">
+      <c r="J13" s="75">
         <v>124316</v>
       </c>
-      <c r="K13" s="89">
+      <c r="K13" s="88">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L13" s="89">
+      <c r="L13" s="88">
         <v>26.9</v>
       </c>
-      <c r="M13" s="90">
+      <c r="M13" s="89">
         <v>36.1</v>
       </c>
-      <c r="N13" s="76">
+      <c r="N13" s="75">
         <v>77069</v>
       </c>
-      <c r="O13" s="89">
+      <c r="O13" s="88">
         <v>5.5</v>
       </c>
-      <c r="P13" s="89">
+      <c r="P13" s="88">
         <v>24.4</v>
       </c>
-      <c r="Q13" s="90">
+      <c r="Q13" s="89">
         <v>38.4</v>
       </c>
-      <c r="R13" s="76">
+      <c r="R13" s="75">
         <v>44689</v>
       </c>
-      <c r="S13" s="89">
+      <c r="S13" s="88">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T13" s="89">
+      <c r="T13" s="88">
         <v>26.6</v>
       </c>
-      <c r="U13" s="90">
+      <c r="U13" s="89">
         <v>45.7</v>
       </c>
-      <c r="V13" s="76">
+      <c r="V13" s="75">
         <v>12242</v>
       </c>
-      <c r="W13" s="89">
+      <c r="W13" s="88">
         <v>3.9</v>
       </c>
-      <c r="X13" s="89">
+      <c r="X13" s="88">
         <v>38.299999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="93">
+      <c r="A14" s="92">
         <v>2008</v>
       </c>
-      <c r="B14" s="76">
+      <c r="B14" s="75">
         <v>99426</v>
       </c>
-      <c r="C14" s="89">
+      <c r="C14" s="137">
         <v>1</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="88">
         <v>43.7</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E14" s="91">
         <v>78.400000000000006</v>
       </c>
-      <c r="F14" s="74">
+      <c r="F14" s="73">
         <v>155537</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="90">
         <v>3.1</v>
       </c>
-      <c r="H14" s="91">
+      <c r="H14" s="90">
         <v>33.799999999999997</v>
       </c>
-      <c r="I14" s="90">
+      <c r="I14" s="89">
         <v>50.4</v>
       </c>
-      <c r="J14" s="76">
+      <c r="J14" s="75">
         <v>119829</v>
       </c>
-      <c r="K14" s="89">
+      <c r="K14" s="88">
         <v>5</v>
       </c>
-      <c r="L14" s="89">
+      <c r="L14" s="88">
         <v>28.5</v>
       </c>
-      <c r="M14" s="90">
+      <c r="M14" s="89">
         <v>35.4</v>
       </c>
-      <c r="N14" s="76">
+      <c r="N14" s="75">
         <v>73315</v>
       </c>
-      <c r="O14" s="89">
+      <c r="O14" s="88">
         <v>5.5</v>
       </c>
-      <c r="P14" s="89">
+      <c r="P14" s="88">
         <v>25.5</v>
       </c>
-      <c r="Q14" s="90">
+      <c r="Q14" s="89">
         <v>37.799999999999997</v>
       </c>
-      <c r="R14" s="76">
+      <c r="R14" s="75">
         <v>43697</v>
       </c>
-      <c r="S14" s="89">
+      <c r="S14" s="88">
         <v>5.2</v>
       </c>
-      <c r="T14" s="89">
+      <c r="T14" s="88">
         <v>27</v>
       </c>
-      <c r="U14" s="90">
+      <c r="U14" s="89">
         <v>44.7</v>
       </c>
-      <c r="V14" s="76">
+      <c r="V14" s="75">
         <v>11835</v>
       </c>
-      <c r="W14" s="89">
+      <c r="W14" s="88">
         <v>4</v>
       </c>
-      <c r="X14" s="89">
+      <c r="X14" s="88">
         <v>39.4</v>
       </c>
     </row>
     <row r="15" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="93">
+      <c r="A15" s="92">
         <v>2007</v>
       </c>
-      <c r="B15" s="76">
+      <c r="B15" s="75">
         <v>91943</v>
       </c>
-      <c r="C15" s="89">
+      <c r="C15" s="137">
         <v>1.2</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D15" s="88">
         <v>44</v>
       </c>
-      <c r="E15" s="92">
+      <c r="E15" s="91">
         <v>77.3</v>
       </c>
-      <c r="F15" s="74">
+      <c r="F15" s="73">
         <v>153587</v>
       </c>
-      <c r="G15" s="91">
+      <c r="G15" s="90">
         <v>3.4</v>
       </c>
-      <c r="H15" s="91">
+      <c r="H15" s="90">
         <v>34.4</v>
       </c>
-      <c r="I15" s="90">
+      <c r="I15" s="89">
         <v>49.7</v>
       </c>
-      <c r="J15" s="76">
+      <c r="J15" s="75">
         <v>116596</v>
       </c>
-      <c r="K15" s="89">
+      <c r="K15" s="88">
         <v>5.3</v>
       </c>
-      <c r="L15" s="89">
+      <c r="L15" s="88">
         <v>29.2</v>
       </c>
-      <c r="M15" s="90">
+      <c r="M15" s="89">
         <v>35.299999999999997</v>
       </c>
-      <c r="N15" s="76">
+      <c r="N15" s="75">
         <v>74713</v>
       </c>
-      <c r="O15" s="89">
+      <c r="O15" s="88">
         <v>5.8</v>
       </c>
-      <c r="P15" s="89">
+      <c r="P15" s="88">
         <v>25.3</v>
       </c>
-      <c r="Q15" s="90">
+      <c r="Q15" s="89">
         <v>38.200000000000003</v>
       </c>
-      <c r="R15" s="76">
+      <c r="R15" s="75">
         <v>4598</v>
       </c>
-      <c r="S15" s="89">
+      <c r="S15" s="88">
         <v>5.4</v>
       </c>
-      <c r="T15" s="89">
+      <c r="T15" s="88">
         <v>27.5</v>
       </c>
-      <c r="U15" s="90">
+      <c r="U15" s="89">
         <v>45.3</v>
       </c>
-      <c r="V15" s="76">
+      <c r="V15" s="75">
         <v>12022</v>
       </c>
-      <c r="W15" s="89">
+      <c r="W15" s="88">
         <v>4.3</v>
       </c>
-      <c r="X15" s="89">
+      <c r="X15" s="88">
         <v>39.6</v>
       </c>
     </row>
     <row r="16" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="93">
+      <c r="A16" s="92">
         <v>2006</v>
       </c>
-      <c r="B16" s="76">
+      <c r="B16" s="75">
         <v>98534</v>
       </c>
-      <c r="C16" s="89">
+      <c r="C16" s="137">
         <v>1.3</v>
       </c>
-      <c r="D16" s="89">
+      <c r="D16" s="88">
         <v>43.5</v>
       </c>
-      <c r="E16" s="92">
+      <c r="E16" s="91">
         <v>76.5</v>
       </c>
-      <c r="F16" s="74">
+      <c r="F16" s="73">
         <v>146178</v>
       </c>
-      <c r="G16" s="91">
+      <c r="G16" s="90">
         <v>3.6</v>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="90">
         <v>35.5</v>
       </c>
-      <c r="I16" s="90">
+      <c r="I16" s="89">
         <v>49.1</v>
       </c>
-      <c r="J16" s="76">
+      <c r="J16" s="75">
         <v>99058</v>
       </c>
-      <c r="K16" s="89">
+      <c r="K16" s="88">
         <v>5.4</v>
       </c>
-      <c r="L16" s="89">
+      <c r="L16" s="88">
         <v>30.9</v>
       </c>
-      <c r="M16" s="90">
+      <c r="M16" s="89">
         <v>35.4</v>
       </c>
-      <c r="N16" s="76">
+      <c r="N16" s="75">
         <v>75304</v>
       </c>
-      <c r="O16" s="89">
+      <c r="O16" s="88">
         <v>6</v>
       </c>
-      <c r="P16" s="89">
+      <c r="P16" s="88">
         <v>27.4</v>
       </c>
-      <c r="Q16" s="90">
+      <c r="Q16" s="89">
         <v>39</v>
       </c>
-      <c r="R16" s="76">
+      <c r="R16" s="75">
         <v>45029</v>
       </c>
-      <c r="S16" s="89">
+      <c r="S16" s="88">
         <v>5.5</v>
       </c>
-      <c r="T16" s="89">
+      <c r="T16" s="88">
         <v>29.6</v>
       </c>
-      <c r="U16" s="90">
+      <c r="U16" s="89">
         <v>46.8</v>
       </c>
-      <c r="V16" s="76">
+      <c r="V16" s="75">
         <v>11932</v>
       </c>
-      <c r="W16" s="89">
+      <c r="W16" s="88">
         <v>4.4000000000000004</v>
       </c>
-      <c r="X16" s="89">
+      <c r="X16" s="88">
         <v>42.9</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="93">
+      <c r="A17" s="92">
         <v>2005</v>
       </c>
-      <c r="B17" s="76">
+      <c r="B17" s="75">
         <v>97243</v>
       </c>
-      <c r="C17" s="89">
+      <c r="C17" s="137">
         <v>1.4</v>
       </c>
-      <c r="D17" s="89">
+      <c r="D17" s="88">
         <v>42</v>
       </c>
-      <c r="E17" s="92">
+      <c r="E17" s="91">
         <v>75.099999999999994</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="73">
         <v>139272</v>
       </c>
-      <c r="G17" s="91">
+      <c r="G17" s="90">
         <v>3.7</v>
       </c>
-      <c r="H17" s="91">
+      <c r="H17" s="90">
         <v>35.700000000000003</v>
       </c>
-      <c r="I17" s="90">
+      <c r="I17" s="89">
         <v>47.9</v>
       </c>
-      <c r="J17" s="76">
+      <c r="J17" s="75">
         <v>91146</v>
       </c>
-      <c r="K17" s="89">
+      <c r="K17" s="88">
         <v>5.6</v>
       </c>
-      <c r="L17" s="89">
+      <c r="L17" s="88">
         <v>31.5</v>
       </c>
-      <c r="M17" s="90">
+      <c r="M17" s="89">
         <v>35.1</v>
       </c>
-      <c r="N17" s="76">
+      <c r="N17" s="75">
         <v>73317</v>
       </c>
-      <c r="O17" s="89">
+      <c r="O17" s="88">
         <v>6.1</v>
       </c>
-      <c r="P17" s="89">
+      <c r="P17" s="88">
         <v>27.7</v>
       </c>
-      <c r="Q17" s="90">
+      <c r="Q17" s="89">
         <v>38.6</v>
       </c>
-      <c r="R17" s="76">
+      <c r="R17" s="75">
         <v>42509</v>
       </c>
-      <c r="S17" s="89">
+      <c r="S17" s="88">
         <v>5.5</v>
       </c>
-      <c r="T17" s="89">
+      <c r="T17" s="88">
         <v>30.6</v>
       </c>
-      <c r="U17" s="90">
+      <c r="U17" s="89">
         <v>46.3</v>
       </c>
-      <c r="V17" s="76">
+      <c r="V17" s="75">
         <v>9918</v>
       </c>
-      <c r="W17" s="89">
+      <c r="W17" s="88">
         <v>4.2</v>
       </c>
-      <c r="X17" s="89">
+      <c r="X17" s="88">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="93">
+      <c r="A18" s="92">
         <v>2004</v>
       </c>
-      <c r="B18" s="76">
+      <c r="B18" s="75">
         <v>95771</v>
       </c>
-      <c r="C18" s="89">
+      <c r="C18" s="137">
         <v>1.7</v>
       </c>
-      <c r="D18" s="89">
+      <c r="D18" s="88">
         <v>42</v>
       </c>
-      <c r="E18" s="92">
+      <c r="E18" s="91">
         <v>74.5</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="73">
         <v>135058</v>
       </c>
-      <c r="G18" s="91">
+      <c r="G18" s="90">
         <v>3.9</v>
       </c>
-      <c r="H18" s="91">
+      <c r="H18" s="90">
         <v>36.5</v>
       </c>
-      <c r="I18" s="90">
+      <c r="I18" s="89">
         <v>47.5</v>
       </c>
-      <c r="J18" s="76">
+      <c r="J18" s="75">
         <v>97353</v>
       </c>
-      <c r="K18" s="89">
+      <c r="K18" s="88">
         <v>6.1</v>
       </c>
-      <c r="L18" s="89">
+      <c r="L18" s="88">
         <v>32.1</v>
       </c>
-      <c r="M18" s="90">
+      <c r="M18" s="89">
         <v>35.1</v>
       </c>
-      <c r="N18" s="76">
+      <c r="N18" s="75">
         <v>73665</v>
       </c>
-      <c r="O18" s="89">
+      <c r="O18" s="88">
         <v>6.6</v>
       </c>
-      <c r="P18" s="89">
+      <c r="P18" s="88">
         <v>27.7</v>
       </c>
-      <c r="Q18" s="90">
+      <c r="Q18" s="89">
         <v>39.1</v>
       </c>
-      <c r="R18" s="76">
+      <c r="R18" s="75">
         <v>41732</v>
       </c>
-      <c r="S18" s="89">
+      <c r="S18" s="88">
         <v>5.9</v>
       </c>
-      <c r="T18" s="89">
+      <c r="T18" s="88">
         <v>31.5</v>
       </c>
-      <c r="U18" s="90">
+      <c r="U18" s="89">
         <v>46.2</v>
       </c>
-      <c r="V18" s="76">
+      <c r="V18" s="75">
         <v>9526</v>
       </c>
-      <c r="W18" s="89">
+      <c r="W18" s="88">
         <v>5</v>
       </c>
-      <c r="X18" s="89">
+      <c r="X18" s="88">
         <v>43.9</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="93">
+      <c r="A19" s="92">
         <v>2003</v>
       </c>
-      <c r="B19" s="76">
+      <c r="B19" s="75">
         <v>93014</v>
       </c>
-      <c r="C19" s="89">
+      <c r="C19" s="137">
         <v>1.9</v>
       </c>
-      <c r="D19" s="89">
+      <c r="D19" s="88">
         <v>42.3</v>
       </c>
-      <c r="E19" s="92">
+      <c r="E19" s="91">
         <v>74</v>
       </c>
-      <c r="F19" s="74">
+      <c r="F19" s="73">
         <v>129643</v>
       </c>
-      <c r="G19" s="91">
+      <c r="G19" s="90">
         <v>4.3</v>
       </c>
-      <c r="H19" s="91">
+      <c r="H19" s="90">
         <v>36.700000000000003</v>
       </c>
-      <c r="I19" s="90">
+      <c r="I19" s="89">
         <v>46.9</v>
       </c>
-      <c r="J19" s="76">
+      <c r="J19" s="75">
         <v>93728</v>
       </c>
-      <c r="K19" s="89">
+      <c r="K19" s="88">
         <v>6.5</v>
       </c>
-      <c r="L19" s="89">
+      <c r="L19" s="88">
         <v>31.9</v>
       </c>
-      <c r="M19" s="90">
+      <c r="M19" s="89">
         <v>35.299999999999997</v>
       </c>
-      <c r="N19" s="76">
+      <c r="N19" s="75">
         <v>73786</v>
       </c>
-      <c r="O19" s="89">
+      <c r="O19" s="88">
         <v>6.9</v>
       </c>
-      <c r="P19" s="89">
+      <c r="P19" s="88">
         <v>28.2</v>
       </c>
-      <c r="Q19" s="90">
+      <c r="Q19" s="89">
         <v>39</v>
       </c>
-      <c r="R19" s="76">
+      <c r="R19" s="75">
         <v>40180</v>
       </c>
-      <c r="S19" s="89">
+      <c r="S19" s="88">
         <v>6.2</v>
       </c>
-      <c r="T19" s="89">
+      <c r="T19" s="88">
         <v>31.8</v>
       </c>
-      <c r="U19" s="90">
+      <c r="U19" s="89">
         <v>45.3</v>
       </c>
-      <c r="V19" s="76">
+      <c r="V19" s="75">
         <v>9490</v>
       </c>
-      <c r="W19" s="89">
+      <c r="W19" s="88">
         <v>4.8</v>
       </c>
-      <c r="X19" s="89">
+      <c r="X19" s="88">
         <v>45.6</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="93">
+      <c r="A20" s="92">
         <v>2002</v>
       </c>
-      <c r="B20" s="76">
+      <c r="B20" s="75">
         <v>9919</v>
       </c>
-      <c r="C20" s="89">
+      <c r="C20" s="137">
         <v>2</v>
       </c>
-      <c r="D20" s="89">
+      <c r="D20" s="88">
         <v>42.1</v>
       </c>
-      <c r="E20" s="92">
+      <c r="E20" s="91">
         <v>72.900000000000006</v>
       </c>
-      <c r="F20" s="74">
+      <c r="F20" s="73">
         <v>122349</v>
       </c>
-      <c r="G20" s="91">
+      <c r="G20" s="90">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H20" s="91">
+      <c r="H20" s="90">
         <v>36.799999999999997</v>
       </c>
-      <c r="I20" s="90">
+      <c r="I20" s="89">
         <v>45.8</v>
       </c>
-      <c r="J20" s="76">
+      <c r="J20" s="75">
         <v>91279</v>
       </c>
-      <c r="K20" s="89">
+      <c r="K20" s="88">
         <v>6.4</v>
       </c>
-      <c r="L20" s="89">
+      <c r="L20" s="88">
         <v>32.200000000000003</v>
       </c>
-      <c r="M20" s="90">
+      <c r="M20" s="89">
         <v>34.6</v>
       </c>
-      <c r="N20" s="76">
+      <c r="N20" s="75">
         <v>70647</v>
       </c>
-      <c r="O20" s="89">
+      <c r="O20" s="88">
         <v>7.1</v>
       </c>
-      <c r="P20" s="89">
+      <c r="P20" s="88">
         <v>28.3</v>
       </c>
-      <c r="Q20" s="90">
+      <c r="Q20" s="89">
         <v>37.9</v>
       </c>
-      <c r="R20" s="76">
+      <c r="R20" s="75">
         <v>37458</v>
       </c>
-      <c r="S20" s="89">
+      <c r="S20" s="88">
         <v>6.4</v>
       </c>
-      <c r="T20" s="89">
+      <c r="T20" s="88">
         <v>31.9</v>
       </c>
-      <c r="U20" s="90">
+      <c r="U20" s="89">
         <v>43.7</v>
       </c>
-      <c r="V20" s="76">
+      <c r="V20" s="75">
         <v>8546</v>
       </c>
-      <c r="W20" s="89">
+      <c r="W20" s="88">
         <v>5.3</v>
       </c>
-      <c r="X20" s="89">
+      <c r="X20" s="88">
         <v>44.2</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="93">
+      <c r="A21" s="92">
         <v>2001</v>
       </c>
-      <c r="B21" s="76">
+      <c r="B21" s="75">
         <v>89703</v>
       </c>
-      <c r="C21" s="89">
+      <c r="C21" s="137">
         <v>2.1</v>
       </c>
-      <c r="D21" s="89">
+      <c r="D21" s="88">
         <v>42.8</v>
       </c>
-      <c r="E21" s="92">
+      <c r="E21" s="91">
         <v>72.099999999999994</v>
       </c>
-      <c r="F21" s="74">
+      <c r="F21" s="73">
         <v>116576</v>
       </c>
-      <c r="G21" s="91">
+      <c r="G21" s="90">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H21" s="91">
+      <c r="H21" s="90">
         <v>38.4</v>
       </c>
-      <c r="I21" s="90">
+      <c r="I21" s="89">
         <v>45.3</v>
       </c>
-      <c r="J21" s="76">
+      <c r="J21" s="75">
         <v>90366</v>
       </c>
-      <c r="K21" s="89">
+      <c r="K21" s="88">
         <v>6.5</v>
       </c>
-      <c r="L21" s="89">
+      <c r="L21" s="88">
         <v>32.9</v>
       </c>
-      <c r="M21" s="90">
+      <c r="M21" s="89">
         <v>33.799999999999997</v>
       </c>
-      <c r="N21" s="76">
+      <c r="N21" s="75">
         <v>66545</v>
       </c>
-      <c r="O21" s="89">
+      <c r="O21" s="88">
         <v>6.9</v>
       </c>
-      <c r="P21" s="89">
+      <c r="P21" s="88">
         <v>29</v>
       </c>
-      <c r="Q21" s="90">
+      <c r="Q21" s="89">
         <v>36.700000000000003</v>
       </c>
-      <c r="R21" s="76">
+      <c r="R21" s="75">
         <v>33851</v>
       </c>
-      <c r="S21" s="89">
+      <c r="S21" s="88">
         <v>6.4</v>
       </c>
-      <c r="T21" s="89">
+      <c r="T21" s="88">
         <v>32.1</v>
       </c>
-      <c r="U21" s="90">
+      <c r="U21" s="89">
         <v>41.4</v>
       </c>
-      <c r="V21" s="76">
+      <c r="V21" s="75">
         <v>7382</v>
       </c>
-      <c r="W21" s="89">
+      <c r="W21" s="88">
         <v>5.6</v>
       </c>
-      <c r="X21" s="89">
+      <c r="X21" s="88">
         <v>42.5</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="93">
+      <c r="A22" s="92">
         <v>2000</v>
       </c>
-      <c r="B22" s="76">
+      <c r="B22" s="75">
         <v>91179</v>
       </c>
-      <c r="C22" s="89">
+      <c r="C22" s="137">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D22" s="89">
+      <c r="D22" s="88">
         <v>41.7</v>
       </c>
-      <c r="E22" s="92">
+      <c r="E22" s="91">
         <v>71.7</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="73">
         <v>113922</v>
       </c>
-      <c r="G22" s="91">
+      <c r="G22" s="90">
         <v>4.8</v>
       </c>
-      <c r="H22" s="91">
+      <c r="H22" s="90">
         <v>37.9</v>
       </c>
-      <c r="I22" s="90">
+      <c r="I22" s="89">
         <v>44.1</v>
       </c>
-      <c r="J22" s="76">
+      <c r="J22" s="75">
         <v>92409</v>
       </c>
-      <c r="K22" s="89">
+      <c r="K22" s="88">
         <v>6.8</v>
       </c>
-      <c r="L22" s="89">
+      <c r="L22" s="88">
         <v>32.4</v>
       </c>
-      <c r="M22" s="90">
+      <c r="M22" s="89">
         <v>33.200000000000003</v>
       </c>
-      <c r="N22" s="76">
+      <c r="N22" s="75">
         <v>64865</v>
       </c>
-      <c r="O22" s="89">
+      <c r="O22" s="88">
         <v>7.3</v>
       </c>
-      <c r="P22" s="89">
+      <c r="P22" s="88">
         <v>29.1</v>
       </c>
-      <c r="Q22" s="90">
+      <c r="Q22" s="89">
         <v>35.700000000000003</v>
       </c>
-      <c r="R22" s="76">
+      <c r="R22" s="75">
         <v>31701</v>
       </c>
-      <c r="S22" s="89">
+      <c r="S22" s="88">
         <v>6.2</v>
       </c>
-      <c r="T22" s="89">
+      <c r="T22" s="88">
         <v>32.5</v>
       </c>
-      <c r="U22" s="90">
+      <c r="U22" s="89">
         <v>39.299999999999997</v>
       </c>
-      <c r="V22" s="76">
+      <c r="V22" s="75">
         <v>6683</v>
       </c>
-      <c r="W22" s="89">
+      <c r="W22" s="88">
         <v>5.6</v>
       </c>
-      <c r="X22" s="89">
+      <c r="X22" s="88">
         <v>43.3</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="93">
+      <c r="A23" s="92">
         <v>1999</v>
       </c>
-      <c r="B23" s="76">
+      <c r="B23" s="75">
         <v>92350</v>
       </c>
-      <c r="C23" s="89">
+      <c r="C23" s="137">
         <v>2.4</v>
       </c>
-      <c r="D23" s="89">
+      <c r="D23" s="88">
         <v>40.799999999999997</v>
       </c>
-      <c r="E23" s="92">
+      <c r="E23" s="91">
         <v>71.099999999999994</v>
       </c>
-      <c r="F23" s="74">
+      <c r="F23" s="73">
         <v>111995</v>
       </c>
-      <c r="G23" s="91">
+      <c r="G23" s="90">
         <v>5</v>
       </c>
-      <c r="H23" s="91">
+      <c r="H23" s="90">
         <v>37.299999999999997</v>
       </c>
-      <c r="I23" s="90">
+      <c r="I23" s="89">
         <v>43.5</v>
       </c>
-      <c r="J23" s="76">
+      <c r="J23" s="75">
         <v>94921</v>
       </c>
-      <c r="K23" s="89">
+      <c r="K23" s="88">
         <v>7.1</v>
       </c>
-      <c r="L23" s="89">
+      <c r="L23" s="88">
         <v>32.4</v>
       </c>
-      <c r="M23" s="90">
+      <c r="M23" s="89">
         <v>32.799999999999997</v>
       </c>
-      <c r="N23" s="76">
+      <c r="N23" s="75">
         <v>64665</v>
       </c>
-      <c r="O23" s="89">
+      <c r="O23" s="88">
         <v>7.7</v>
       </c>
-      <c r="P23" s="89">
+      <c r="P23" s="88">
         <v>29.2</v>
       </c>
-      <c r="Q23" s="90">
+      <c r="Q23" s="89">
         <v>35.1</v>
       </c>
-      <c r="R23" s="76">
+      <c r="R23" s="75">
         <v>30182</v>
       </c>
-      <c r="S23" s="89">
+      <c r="S23" s="88">
         <v>7</v>
       </c>
-      <c r="T23" s="89">
+      <c r="T23" s="88">
         <v>33</v>
       </c>
-      <c r="U23" s="90">
+      <c r="U23" s="89">
         <v>39.5</v>
       </c>
-      <c r="V23" s="76">
+      <c r="V23" s="75">
         <v>6331</v>
       </c>
-      <c r="W23" s="89">
+      <c r="W23" s="88">
         <v>5.6</v>
       </c>
-      <c r="X23" s="89">
+      <c r="X23" s="88">
         <v>43.9</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="93">
+      <c r="A24" s="92">
         <v>1998</v>
       </c>
-      <c r="B24" s="76">
+      <c r="B24" s="75">
         <v>94890</v>
       </c>
-      <c r="C24" s="89">
+      <c r="C24" s="137">
         <v>2.6</v>
       </c>
-      <c r="D24" s="89">
+      <c r="D24" s="88">
         <v>40</v>
       </c>
-      <c r="E24" s="92">
+      <c r="E24" s="91">
         <v>70.099999999999994</v>
       </c>
-      <c r="F24" s="74">
+      <c r="F24" s="73">
         <v>114382</v>
       </c>
-      <c r="G24" s="91">
+      <c r="G24" s="90">
         <v>5.5</v>
       </c>
-      <c r="H24" s="91">
+      <c r="H24" s="90">
         <v>36.9</v>
       </c>
-      <c r="I24" s="90">
+      <c r="I24" s="89">
         <v>42.7</v>
       </c>
-      <c r="J24" s="76">
+      <c r="J24" s="75">
         <v>9929</v>
       </c>
-      <c r="K24" s="89">
+      <c r="K24" s="88">
         <v>7.6</v>
       </c>
-      <c r="L24" s="89">
+      <c r="L24" s="88">
         <v>32.1</v>
       </c>
-      <c r="M24" s="90">
+      <c r="M24" s="89">
         <v>32.299999999999997</v>
       </c>
-      <c r="N24" s="76">
+      <c r="N24" s="75">
         <v>65074</v>
       </c>
-      <c r="O24" s="89">
+      <c r="O24" s="88">
         <v>7.9</v>
       </c>
-      <c r="P24" s="89">
+      <c r="P24" s="88">
         <v>29.2</v>
       </c>
-      <c r="Q24" s="90">
+      <c r="Q24" s="89">
         <v>34.700000000000003</v>
       </c>
-      <c r="R24" s="76">
+      <c r="R24" s="75">
         <v>28727</v>
       </c>
-      <c r="S24" s="89">
+      <c r="S24" s="88">
         <v>7.6</v>
       </c>
-      <c r="T24" s="89">
+      <c r="T24" s="88">
         <v>33.299999999999997</v>
       </c>
-      <c r="U24" s="90">
+      <c r="U24" s="89">
         <v>38.200000000000003</v>
       </c>
-      <c r="V24" s="76">
+      <c r="V24" s="75">
         <v>5873</v>
       </c>
-      <c r="W24" s="89">
+      <c r="W24" s="88">
         <v>6</v>
       </c>
-      <c r="X24" s="89">
+      <c r="X24" s="88">
         <v>44.7</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
+      <c r="A25" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -13142,86 +13027,86 @@
   </sheetPr>
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.84375" style="70" customWidth="1"/>
-    <col min="2" max="2" width="12.84375" style="70" customWidth="1"/>
-    <col min="3" max="20" width="17.4609375" style="104" customWidth="1"/>
-    <col min="21" max="16384" width="8.84375" style="70"/>
+    <col min="1" max="1" width="40.84375" style="69" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="69" customWidth="1"/>
+    <col min="3" max="20" width="17.4609375" style="103" customWidth="1"/>
+    <col min="21" max="16384" width="8.84375" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="74.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="104" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="C1" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="D1" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="109" t="s">
+      <c r="F1" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="110" t="s">
+      <c r="G1" s="110" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="111" t="s">
+      <c r="H1" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="110" t="s">
+      <c r="I1" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="112" t="s">
+      <c r="J1" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="108" t="s">
+      <c r="K1" s="110" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="111" t="s">
+      <c r="L1" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="110" t="s">
+      <c r="M1" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="113" t="s">
+      <c r="N1" s="109" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="110" t="s">
+      <c r="O1" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="114" t="s">
+      <c r="P1" s="109" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="110" t="s">
+      <c r="Q1" s="110" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="133" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="110" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="133" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="87" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="111" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="137" t="s">
-        <v>101</v>
-      </c>
-      <c r="S1" s="111" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="137" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="88" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="75" t="s">
+      <c r="B2" s="114" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="115" t="s">
-        <v>87</v>
       </c>
       <c r="C2" s="16">
         <v>817515</v>
@@ -13229,7 +13114,7 @@
       <c r="D2" s="55">
         <v>25.3</v>
       </c>
-      <c r="E2" s="98">
+      <c r="E2" s="97">
         <v>2085</v>
       </c>
       <c r="F2" s="55">
@@ -13250,7 +13135,7 @@
       <c r="K2" s="16">
         <v>138373</v>
       </c>
-      <c r="L2" s="97">
+      <c r="L2" s="96">
         <v>38</v>
       </c>
       <c r="M2" s="16">
@@ -13265,25 +13150,25 @@
       <c r="P2" s="55">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q2" s="116">
+      <c r="Q2" s="115">
         <v>132113</v>
       </c>
-      <c r="R2" s="117">
+      <c r="R2" s="116">
         <v>21.4</v>
       </c>
-      <c r="S2" s="116">
+      <c r="S2" s="115">
         <v>31438</v>
       </c>
-      <c r="T2" s="117">
+      <c r="T2" s="116">
         <v>34.1</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="71" t="s">
-        <v>88</v>
+      <c r="A3" s="70" t="s">
+        <v>87</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="22">
         <v>780013</v>
@@ -13327,25 +13212,25 @@
       <c r="P3" s="20">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q3" s="118">
+      <c r="Q3" s="117">
         <v>127123</v>
       </c>
-      <c r="R3" s="119">
+      <c r="R3" s="118">
         <v>21.3</v>
       </c>
-      <c r="S3" s="118">
+      <c r="S3" s="117">
         <v>30421</v>
       </c>
-      <c r="T3" s="120">
+      <c r="T3" s="119">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
-        <v>89</v>
+      <c r="A4" s="70" t="s">
+        <v>88</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="22">
         <v>37500</v>
@@ -13389,25 +13274,25 @@
       <c r="P4" s="20">
         <v>18.3</v>
       </c>
-      <c r="Q4" s="118">
+      <c r="Q4" s="117">
         <v>4988</v>
       </c>
-      <c r="R4" s="119">
+      <c r="R4" s="118">
         <v>22.3</v>
       </c>
-      <c r="S4" s="118">
+      <c r="S4" s="117">
         <v>1017</v>
       </c>
-      <c r="T4" s="119">
+      <c r="T4" s="118">
         <v>37.799999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="94" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" s="95" t="s">
-        <v>91</v>
       </c>
       <c r="C5" s="22">
         <v>32664</v>
@@ -13451,25 +13336,25 @@
       <c r="P5" s="20">
         <v>18.2</v>
       </c>
-      <c r="Q5" s="118">
+      <c r="Q5" s="117">
         <v>4168</v>
       </c>
-      <c r="R5" s="119">
+      <c r="R5" s="118">
         <v>21.8</v>
       </c>
-      <c r="S5" s="118">
+      <c r="S5" s="117">
         <v>891</v>
       </c>
-      <c r="T5" s="119">
+      <c r="T5" s="118">
         <v>34.799999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="95" t="s">
+      <c r="A6" s="70" t="s">
         <v>91</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C6" s="22">
         <v>106406</v>
@@ -13513,25 +13398,25 @@
       <c r="P6" s="20">
         <v>19.7</v>
       </c>
-      <c r="Q6" s="118">
+      <c r="Q6" s="117">
         <v>15191</v>
       </c>
-      <c r="R6" s="120">
+      <c r="R6" s="119">
         <v>23</v>
       </c>
-      <c r="S6" s="118">
+      <c r="S6" s="117">
         <v>3343</v>
       </c>
-      <c r="T6" s="119">
+      <c r="T6" s="118">
         <v>36.299999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="95" t="s">
-        <v>91</v>
+      <c r="A7" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C7" s="22">
         <v>72721</v>
@@ -13575,25 +13460,25 @@
       <c r="P7" s="20">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q7" s="118">
+      <c r="Q7" s="117">
         <v>9792</v>
       </c>
-      <c r="R7" s="120">
+      <c r="R7" s="119">
         <v>22</v>
       </c>
-      <c r="S7" s="118">
+      <c r="S7" s="117">
         <v>2193</v>
       </c>
-      <c r="T7" s="119">
+      <c r="T7" s="118">
         <v>32.700000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="95" t="s">
-        <v>91</v>
+      <c r="A8" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C8" s="22">
         <v>61113</v>
@@ -13637,25 +13522,25 @@
       <c r="P8" s="58">
         <v>17</v>
       </c>
-      <c r="Q8" s="118">
+      <c r="Q8" s="117">
         <v>8462</v>
       </c>
-      <c r="R8" s="119">
+      <c r="R8" s="118">
         <v>21.8</v>
       </c>
-      <c r="S8" s="118">
+      <c r="S8" s="117">
         <v>1970</v>
       </c>
-      <c r="T8" s="119">
+      <c r="T8" s="118">
         <v>35.5</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="95" t="s">
-        <v>91</v>
+      <c r="A9" s="70" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C9" s="22">
         <v>85850</v>
@@ -13699,25 +13584,25 @@
       <c r="P9" s="20">
         <v>19.899999999999999</v>
       </c>
-      <c r="Q9" s="118">
+      <c r="Q9" s="117">
         <v>12097</v>
       </c>
-      <c r="R9" s="119">
+      <c r="R9" s="118">
         <v>25.1</v>
       </c>
-      <c r="S9" s="118">
+      <c r="S9" s="117">
         <v>2897</v>
       </c>
-      <c r="T9" s="119">
+      <c r="T9" s="118">
         <v>37.200000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="95" t="s">
-        <v>91</v>
+      <c r="A10" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C10" s="22">
         <v>84421</v>
@@ -13761,25 +13646,25 @@
       <c r="P10" s="20">
         <v>15.3</v>
       </c>
-      <c r="Q10" s="118">
+      <c r="Q10" s="117">
         <v>13967</v>
       </c>
-      <c r="R10" s="119">
+      <c r="R10" s="118">
         <v>20.7</v>
       </c>
-      <c r="S10" s="118">
+      <c r="S10" s="117">
         <v>3147</v>
       </c>
-      <c r="T10" s="119">
+      <c r="T10" s="118">
         <v>35.6</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="95" t="s">
-        <v>91</v>
+      <c r="A11" s="70" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="22">
         <v>150871</v>
@@ -13823,25 +13708,25 @@
       <c r="P11" s="20">
         <v>18.899999999999999</v>
       </c>
-      <c r="Q11" s="118">
+      <c r="Q11" s="117">
         <v>31585</v>
       </c>
-      <c r="R11" s="119">
+      <c r="R11" s="118">
         <v>20.8</v>
       </c>
-      <c r="S11" s="118">
+      <c r="S11" s="117">
         <v>8608</v>
       </c>
-      <c r="T11" s="119">
+      <c r="T11" s="118">
         <v>32.299999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="95" t="s">
-        <v>91</v>
+      <c r="A12" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C12" s="22">
         <v>120175</v>
@@ -13885,25 +13770,25 @@
       <c r="P12" s="20">
         <v>15.1</v>
       </c>
-      <c r="Q12" s="118">
+      <c r="Q12" s="117">
         <v>21247</v>
       </c>
-      <c r="R12" s="119">
+      <c r="R12" s="118">
         <v>19.899999999999999</v>
       </c>
-      <c r="S12" s="118">
+      <c r="S12" s="117">
         <v>5078</v>
       </c>
-      <c r="T12" s="119">
+      <c r="T12" s="118">
         <v>33.4</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="95" t="s">
-        <v>91</v>
+      <c r="A13" s="70" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="C13" s="22">
         <v>65792</v>
@@ -13947,16 +13832,16 @@
       <c r="P13" s="20">
         <v>14.7</v>
       </c>
-      <c r="Q13" s="118">
+      <c r="Q13" s="117">
         <v>10614</v>
       </c>
-      <c r="R13" s="119">
+      <c r="R13" s="118">
         <v>18.7</v>
       </c>
-      <c r="S13" s="118">
+      <c r="S13" s="117">
         <v>2294</v>
       </c>
-      <c r="T13" s="119">
+      <c r="T13" s="118">
         <v>31.5</v>
       </c>
     </row>

</xml_diff>